<commit_message>
Added analysis of lorentz's distribution
</commit_message>
<xml_diff>
--- a/oscillazioni/molla.xlsx
+++ b/oscillazioni/molla.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="911" documentId="13_ncr:1_{19EF7A93-7410-479C-B5A9-9683ABBE8874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ED812FC9-2D39-4D4A-9C3B-558B8C837BD0}"/>
+  <xr:revisionPtr revIDLastSave="1008" documentId="13_ncr:1_{19EF7A93-7410-479C-B5A9-9683ABBE8874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C39044F3-4487-43D3-9711-E27C90CE765D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Statico - Calibro" sheetId="1" r:id="rId1"/>
@@ -717,10 +717,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.000000%"/>
+    <numFmt numFmtId="168" formatCode="0.00000000000000"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -831,7 +832,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -945,11 +946,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1062,13 +1087,26 @@
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1352,14 +1390,14 @@
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="4.5703125" customWidth="1"/>
     <col min="12" max="12" width="9.140625" customWidth="1"/>
-    <col min="13" max="13" width="13.7109375" customWidth="1"/>
+    <col min="13" max="13" width="35.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -1408,8 +1446,8 @@
         <v>11</v>
       </c>
       <c r="E2" s="6">
-        <f>162.14+179.81</f>
-        <v>341.95</v>
+        <f>161.14+179.81</f>
+        <v>340.95</v>
       </c>
       <c r="F2" s="6">
         <f>162.2+179.81</f>
@@ -1421,11 +1459,11 @@
       </c>
       <c r="H2" s="6">
         <f t="shared" ref="H2:H9" si="0">AVERAGE(E2,F2,G2)</f>
-        <v>341.92333333333335</v>
+        <v>341.59</v>
       </c>
       <c r="I2" s="14">
         <f t="shared" ref="I2:I9" si="1">_xlfn.STDEV.S(E2,F2,G2)/SQRT(3)</f>
-        <v>5.9254629448766805E-2</v>
+        <v>0.3251666239535273</v>
       </c>
       <c r="J2" s="17" t="s">
         <v>12</v>
@@ -1436,9 +1474,9 @@
       <c r="L2" s="5">
         <v>0</v>
       </c>
-      <c r="M2" s="25">
-        <f>B14*SUM(A4:A7)/(H3-H7)</f>
-        <v>3.7846986256572208</v>
+      <c r="M2" s="59">
+        <f>B14*SUM(A4:A9)/(H3-H9)</f>
+        <v>4.0308227440028572</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -1473,11 +1511,11 @@
       </c>
       <c r="J3" s="18">
         <f>H2-H3</f>
-        <v>39.913333333333355</v>
+        <v>39.579999999999984</v>
       </c>
       <c r="K3" s="18">
         <f>SQRT(POWER(I2,2)+POWER(I3,2))</f>
-        <v>0.54373196010942659</v>
+        <v>0.63076672920079024</v>
       </c>
       <c r="L3" s="5">
         <v>1</v>
@@ -1515,11 +1553,11 @@
       </c>
       <c r="J4" s="18">
         <f>H2-H4</f>
-        <v>81.653333333333364</v>
+        <v>81.319999999999993</v>
       </c>
       <c r="K4" s="18">
         <f>SQRT(POWER(I2,2)+POWER(I4,2))</f>
-        <v>0.46380072349136037</v>
+        <v>0.56332347131406957</v>
       </c>
       <c r="L4" s="5">
         <v>2</v>
@@ -1557,11 +1595,11 @@
       </c>
       <c r="J5" s="18">
         <f>H2-H5</f>
-        <v>123.81333333333336</v>
+        <v>123.47999999999999</v>
       </c>
       <c r="K5" s="18">
         <f>SQRT(POWER(I2,2)+POWER(I5,2))</f>
-        <v>0.53358327476703415</v>
+        <v>0.62203965575623565</v>
       </c>
       <c r="L5" s="5">
         <v>3</v>
@@ -1596,11 +1634,11 @@
       </c>
       <c r="J6" s="18">
         <f>H2-H6</f>
-        <v>202.91000000000003</v>
+        <v>202.57666666666665</v>
       </c>
       <c r="K6" s="39">
         <f>SQRT(POWER(I2,2)+POWER(I6,2))</f>
-        <v>0.11981467170407056</v>
+        <v>0.34143488072805067</v>
       </c>
       <c r="L6" s="5">
         <v>4</v>
@@ -1635,11 +1673,11 @@
       </c>
       <c r="J7" s="18">
         <f>H2-H7</f>
-        <v>244.69</v>
+        <v>244.35666666666663</v>
       </c>
       <c r="K7" s="39">
         <f>SQRT(POWER(I2,2)+POWER(I7,2))</f>
-        <v>0.13399834161494448</v>
+        <v>0.3466666666666689</v>
       </c>
       <c r="L7" s="5">
         <v>5</v>
@@ -1674,11 +1712,11 @@
       </c>
       <c r="J8" s="18">
         <f>H2-H8</f>
-        <v>286.55</v>
+        <v>286.21666666666664</v>
       </c>
       <c r="K8" s="39">
         <f>SQRT(POWER(I2,2)+POWER(I8,2))</f>
-        <v>0.15129074290546912</v>
+        <v>0.35371049053019721</v>
       </c>
       <c r="L8" s="5">
         <v>6</v>
@@ -1716,11 +1754,11 @@
       </c>
       <c r="J9" s="18">
         <f>H2-H9</f>
-        <v>329.35666666666668</v>
+        <v>329.02333333333331</v>
       </c>
       <c r="K9" s="39">
         <f>SQRT(POWER(I2,2)+POWER(I9,2))</f>
-        <v>0.13399834161494367</v>
+        <v>0.34666666666666862</v>
       </c>
       <c r="L9" s="5">
         <v>7</v>
@@ -1800,18 +1838,18 @@
         <v>28.64</v>
       </c>
       <c r="F12" s="6">
-        <v>28.8</v>
+        <v>27.8</v>
       </c>
       <c r="G12" s="6">
         <v>28.58</v>
       </c>
       <c r="H12" s="6">
         <f t="shared" ref="H12:H19" si="2">AVERAGE(E12,F12,G12)</f>
-        <v>28.673333333333332</v>
+        <v>28.34</v>
       </c>
       <c r="I12" s="14">
         <f t="shared" ref="I12:I19" si="3">_xlfn.STDEV.S(E12,F12,G12)/SQRT(3)</f>
-        <v>6.5659052011974625E-2</v>
+        <v>0.27055498516937326</v>
       </c>
       <c r="J12" s="17" t="s">
         <v>12</v>
@@ -1847,11 +1885,11 @@
       </c>
       <c r="J13" s="18">
         <f>H13-H12</f>
-        <v>24.54</v>
+        <v>24.873333333333331</v>
       </c>
       <c r="K13" s="39">
         <f>SQRT(POWER(I12,2)+POWER(I13,2))</f>
-        <v>0.12578641509408861</v>
+        <v>0.2910517327059074</v>
       </c>
       <c r="L13" s="5">
         <v>2</v>
@@ -1883,11 +1921,11 @@
       </c>
       <c r="J14" s="18">
         <f>H14-H12</f>
-        <v>50.16</v>
+        <v>50.493333333333325</v>
       </c>
       <c r="K14" s="18">
         <f>SQRT(POWER(I12,2)+POWER(I14,2))</f>
-        <v>0.38998575472558833</v>
+        <v>0.47008273503477588</v>
       </c>
       <c r="L14" s="5">
         <v>3</v>
@@ -1913,11 +1951,11 @@
       </c>
       <c r="J15" s="18">
         <f>H15-H12</f>
-        <v>74.793333333333322</v>
+        <v>75.126666666666651</v>
       </c>
       <c r="K15" s="18">
         <f>SQRT(POWER(I12,2)+POWER(I15,2))</f>
-        <v>0.26849374087469857</v>
+        <v>0.37547007574210012</v>
       </c>
       <c r="L15" s="5">
         <v>4</v>
@@ -1943,11 +1981,11 @@
       </c>
       <c r="J16" s="18">
         <f>H16-H12</f>
-        <v>101.82666666666667</v>
+        <v>102.16</v>
       </c>
       <c r="K16" s="18">
         <f>SQRT(POWER(I12,2)+POWER(I16,2))</f>
-        <v>0.40944406754091417</v>
+        <v>0.48634692692905679</v>
       </c>
       <c r="L16" s="5">
         <v>5</v>
@@ -1973,11 +2011,11 @@
       </c>
       <c r="J17" s="18">
         <f>H17-H12</f>
-        <v>125.10666666666667</v>
+        <v>125.44</v>
       </c>
       <c r="K17" s="39">
         <f>SQRT(POWER(I12,2)+POWER(I17,2))</f>
-        <v>0.10022197585582447</v>
+        <v>0.280950766742741</v>
       </c>
       <c r="L17" s="5">
         <v>6</v>
@@ -2003,11 +2041,11 @@
       </c>
       <c r="J18" s="18">
         <f>H18-H12</f>
-        <v>151.15333333333336</v>
+        <v>151.48666666666668</v>
       </c>
       <c r="K18" s="39">
         <f>SQRT(POWER(I12,2)+POWER(I18,2))</f>
-        <v>0.10498677165349049</v>
+        <v>0.28268553396152191</v>
       </c>
       <c r="L18" s="5">
         <v>7</v>
@@ -2033,11 +2071,11 @@
       </c>
       <c r="J19" s="18">
         <f>H19-H12</f>
-        <v>177.72000000000003</v>
+        <v>178.05333333333334</v>
       </c>
       <c r="K19" s="39">
         <f>SQRT(POWER(I12,2)+POWER(I19,2))</f>
-        <v>0.12525529485370462</v>
+        <v>0.29082258814916195</v>
       </c>
       <c r="L19" s="5">
         <v>8</v>
@@ -2053,8 +2091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2D4EB93-7770-4A45-A697-00620671C631}">
   <dimension ref="A1:AE381"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView topLeftCell="J1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13992,7 +14030,7 @@
   <dimension ref="A1:AD454"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24398,8 +24436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B459E249-CE69-4C2B-8F77-71C2DA9D2D63}">
   <dimension ref="A1:Y18"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="R17" sqref="R17"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24443,11 +24481,11 @@
         <v>48</v>
       </c>
       <c r="L1" s="13" cm="1">
-        <f t="array" ref="L1:M5">LINEST(G2:G8,E2:E8,TRUE,TRUE)</f>
-        <v>0.39324308915728373</v>
+        <f t="array" ref="L1:M5">LINEST(G2:G9,E2:E9,TRUE,TRUE)</f>
+        <v>0.48213257339934595</v>
       </c>
       <c r="M1" s="13">
-        <v>5.6659979234020739</v>
+        <v>0.60272555380251447</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>49</v>
@@ -24471,11 +24509,11 @@
         <v>48</v>
       </c>
       <c r="W1" s="13" cm="1">
-        <f t="array" ref="W1:X5">LINEST(R2:R8,P2:P8,TRUE,TRUE)</f>
-        <v>0.3784185430642788</v>
+        <f t="array" ref="W1:X5">LINEST(R2:R9,P2:P9,TRUE,TRUE)</f>
+        <v>0.4650553566833357</v>
       </c>
       <c r="X1" s="13">
-        <v>6.9032845362168729</v>
+        <v>1.7017457893045247</v>
       </c>
       <c r="Y1" s="1" t="s">
         <v>49</v>
@@ -24503,11 +24541,11 @@
       </c>
       <c r="H2" s="49">
         <f>F2*B14/B13</f>
-        <v>0.20840362671528331</v>
+        <v>0.22195639906487186</v>
       </c>
       <c r="I2" s="45">
         <f>POWER((G2-E2*L1-M1)/H2,2)</f>
-        <v>53.921183875501264</v>
+        <v>4.3485311504757812E-3</v>
       </c>
       <c r="J2" s="5">
         <v>1</v>
@@ -24516,10 +24554,10 @@
         <v>50</v>
       </c>
       <c r="L2" s="13">
-        <v>1.6334644882533948E-2</v>
+        <v>2.7094215018778501E-3</v>
       </c>
       <c r="M2" s="13">
-        <v>3.4663278947824034</v>
+        <v>0.55929892346831012</v>
       </c>
       <c r="N2" s="23" t="s">
         <v>51</v>
@@ -24536,11 +24574,11 @@
       </c>
       <c r="S2" s="25">
         <f>Q2*B14/B13</f>
-        <v>7.718652841306789E-2</v>
+        <v>8.2206073727730311E-2</v>
       </c>
       <c r="T2" s="45">
         <f>POWER((R2-P2*W1-X1)/S2,2)</f>
-        <v>538.01918463467973</v>
+        <v>0.25838109151036698</v>
       </c>
       <c r="U2" s="5">
         <v>1</v>
@@ -24549,10 +24587,10 @@
         <v>50</v>
       </c>
       <c r="W2" s="13">
-        <v>1.7807719260001832E-2</v>
+        <v>9.5487284759073106E-4</v>
       </c>
       <c r="X2" s="13">
-        <v>3.8746823163353916</v>
+        <v>0.20235481781272108</v>
       </c>
       <c r="Y2" s="23" t="s">
         <v>51</v>
@@ -24580,20 +24618,20 @@
       </c>
       <c r="H3" s="50">
         <f>F3*B14/B13</f>
-        <v>0.17752901535005616</v>
+        <v>0.18907396957377973</v>
       </c>
       <c r="I3" s="45">
         <f>POWER((G3-E3*L1-M1)/H3,2)</f>
-        <v>106.92187042969883</v>
+        <v>3.6021586176783518</v>
       </c>
       <c r="J3" s="5">
         <v>2</v>
       </c>
       <c r="L3" s="13">
-        <v>0.99144664400820359</v>
+        <v>0.99981055237513417</v>
       </c>
       <c r="M3" s="13">
-        <v>4.3366836652646841</v>
+        <v>0.72251141855881962</v>
       </c>
       <c r="P3" s="20">
         <v>80.841999999999999</v>
@@ -24607,20 +24645,20 @@
       </c>
       <c r="S3" s="28">
         <f>Q3*B14/B13</f>
-        <v>7.718652841306789E-2</v>
+        <v>8.2206073727730311E-2</v>
       </c>
       <c r="T3" s="45">
         <f>POWER((R3-P3*W1-X1)/S3,2)</f>
-        <v>750.54186161439429</v>
+        <v>14.427612941388384</v>
       </c>
       <c r="U3" s="5">
         <v>2</v>
       </c>
       <c r="W3" s="13">
-        <v>0.9890488549600539</v>
+        <v>0.99997470573576774</v>
       </c>
       <c r="X3" s="13">
-        <v>4.9070359046895202</v>
+        <v>0.2639995822163822</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
@@ -24633,32 +24671,32 @@
       <c r="C4" s="5">
         <v>2</v>
       </c>
-      <c r="E4" s="20">
+      <c r="E4" s="32">
         <v>123.81</v>
       </c>
-      <c r="F4" s="18">
+      <c r="F4" s="60">
         <v>0.53</v>
       </c>
-      <c r="G4" s="30">
+      <c r="G4" s="61">
         <f>SUM(A3:A5)</f>
         <v>59.370000000000005</v>
       </c>
-      <c r="H4" s="49">
+      <c r="H4" s="62">
         <f>F4*B14/B13</f>
-        <v>0.20454430029462989</v>
-      </c>
-      <c r="I4" s="45">
+        <v>0.21784609537848534</v>
+      </c>
+      <c r="I4" s="63">
         <f>POWER((G4-E4*L1-M1)/H4,2)</f>
-        <v>601.50589869721784</v>
+        <v>18.051325346068662</v>
       </c>
       <c r="J4" s="5">
         <v>3</v>
       </c>
       <c r="L4" s="13">
-        <v>579.5658715474483</v>
+        <v>31665.022554382478</v>
       </c>
       <c r="M4" s="13">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P4" s="20">
         <v>124.02</v>
@@ -24672,20 +24710,20 @@
       </c>
       <c r="S4" s="25">
         <f>Q4*B14/B13</f>
-        <v>7.718652841306789E-2</v>
+        <v>8.2206073727730311E-2</v>
       </c>
       <c r="T4" s="45">
         <f>POWER((R4-P4*W1-X1)/S4,2)</f>
-        <v>5142.6990714977137</v>
+        <v>9.2612306360068865E-3</v>
       </c>
       <c r="U4" s="5">
         <v>3</v>
       </c>
       <c r="W4" s="13">
-        <v>451.57326076512078</v>
+        <v>237201.92765145932</v>
       </c>
       <c r="X4" s="13">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -24698,59 +24736,59 @@
       <c r="C5" s="5">
         <v>3</v>
       </c>
-      <c r="E5" s="20">
-        <v>202.91</v>
-      </c>
-      <c r="F5" s="39">
-        <v>0.2</v>
-      </c>
-      <c r="G5" s="30">
+      <c r="E5" s="6">
+        <v>160.23500000000001</v>
+      </c>
+      <c r="F5" s="69">
+        <v>0.42</v>
+      </c>
+      <c r="G5" s="4">
         <f>SUM(A3:A6)</f>
         <v>79.080000000000013</v>
       </c>
-      <c r="H5" s="49">
+      <c r="H5" s="6">
         <f>F5*B14/B13</f>
-        <v>7.718652841306789E-2</v>
-      </c>
-      <c r="I5" s="45">
+        <v>0.17263275482823368</v>
+      </c>
+      <c r="I5" s="63">
         <f>POWER((G5-E5*L1-M1)/H5,2)</f>
-        <v>6829.9230023834316</v>
+        <v>50.169196318489277</v>
       </c>
       <c r="J5" s="5">
         <v>4</v>
       </c>
       <c r="L5" s="13">
-        <v>10899.794045365707</v>
+        <v>16529.862151000318</v>
       </c>
       <c r="M5" s="13">
-        <v>94.034126062867671</v>
+        <v>3.1321364996872672</v>
       </c>
       <c r="P5" s="20">
-        <v>209.47800000000001</v>
+        <v>166.953</v>
       </c>
       <c r="Q5" s="39">
         <v>0.2</v>
       </c>
       <c r="R5" s="30">
-        <f>SUM(A3:A6)</f>
-        <v>79.080000000000013</v>
+        <f>SUM(A2:A5)</f>
+        <v>79.11</v>
       </c>
       <c r="S5" s="25">
         <f>Q5*B14/B13</f>
-        <v>7.718652841306789E-2</v>
+        <v>8.2206073727730311E-2</v>
       </c>
       <c r="T5" s="45">
         <f>POWER((R5-P5*W1-X1)/S5,2)</f>
-        <v>8446.0913494285141</v>
+        <v>8.1117869074478541</v>
       </c>
       <c r="U5" s="5">
         <v>4</v>
       </c>
       <c r="W5" s="13">
-        <v>10873.433164579015</v>
+        <v>16531.973225323542</v>
       </c>
       <c r="X5" s="13">
-        <v>120.39500684956047</v>
+        <v>0.41817467646254597</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
@@ -24763,29 +24801,29 @@
       <c r="C6" s="5">
         <v>4</v>
       </c>
-      <c r="E6" s="20">
-        <v>244.69</v>
-      </c>
-      <c r="F6" s="39">
-        <v>0.2</v>
-      </c>
-      <c r="G6" s="30">
+      <c r="E6" s="64">
+        <v>202.91</v>
+      </c>
+      <c r="F6" s="65">
+        <v>0.34</v>
+      </c>
+      <c r="G6" s="66">
         <f>SUM(A3:A7)</f>
         <v>98.860000000000014</v>
       </c>
-      <c r="H6" s="49">
+      <c r="H6" s="67">
         <f>F6*B14/B13</f>
-        <v>7.718652841306789E-2</v>
-      </c>
-      <c r="I6" s="45">
+        <v>0.13975032533714155</v>
+      </c>
+      <c r="I6" s="68">
         <f>POWER((G6-E6*L1-M1)/H6,2)</f>
-        <v>1539.6251250591977</v>
+        <v>9.368767434816105</v>
       </c>
       <c r="J6" s="5">
         <v>5</v>
       </c>
       <c r="P6" s="20">
-        <v>252.197</v>
+        <v>209.47800000000001</v>
       </c>
       <c r="Q6" s="39">
         <v>0.2</v>
@@ -24796,11 +24834,11 @@
       </c>
       <c r="S6" s="25">
         <f>Q6*B14/B13</f>
-        <v>7.718652841306789E-2</v>
+        <v>8.2206073727730311E-2</v>
       </c>
       <c r="T6" s="45">
         <f>POWER((R6-P6*W1-X1)/S6,2)</f>
-        <v>2031.899370853343</v>
+        <v>10.050330139642826</v>
       </c>
       <c r="U6" s="5">
         <v>5</v>
@@ -24817,10 +24855,10 @@
         <v>5</v>
       </c>
       <c r="E7" s="20">
-        <v>286.55</v>
+        <v>244.69</v>
       </c>
       <c r="F7" s="39">
-        <v>0.2</v>
+        <v>0.35</v>
       </c>
       <c r="G7" s="30">
         <f>SUM(A3:A8)</f>
@@ -24828,11 +24866,11 @@
       </c>
       <c r="H7" s="49">
         <f>F7*B14/B13</f>
-        <v>7.718652841306789E-2</v>
+        <v>0.14386062902352806</v>
       </c>
       <c r="I7" s="45">
         <f>POWER((G7-E7*L1-M1)/H7,2)</f>
-        <v>37.108446394266977</v>
+        <v>2.8827251219975025</v>
       </c>
       <c r="J7" s="5">
         <v>6</v>
@@ -24842,12 +24880,12 @@
       </c>
       <c r="M7" s="20">
         <f>L1*B13</f>
-        <v>3.8563894754224934</v>
-      </c>
-      <c r="P7" s="32">
-        <v>294.983</v>
-      </c>
-      <c r="Q7" s="47">
+        <v>4.7280957582752281</v>
+      </c>
+      <c r="P7" s="20">
+        <v>252.197</v>
+      </c>
+      <c r="Q7" s="39">
         <v>0.2</v>
       </c>
       <c r="R7" s="30">
@@ -24856,11 +24894,11 @@
       </c>
       <c r="S7" s="25">
         <f>Q7*B14/B13</f>
-        <v>7.718652841306789E-2</v>
+        <v>8.2206073727730311E-2</v>
       </c>
       <c r="T7" s="45">
         <f>POWER((R7-P7*W1-X1)/S7,2)</f>
-        <v>14.084749738259189</v>
+        <v>4.1423251165223745</v>
       </c>
       <c r="U7" s="5">
         <v>6</v>
@@ -24870,7 +24908,7 @@
       </c>
       <c r="X7" s="20">
         <f>W1*B13</f>
-        <v>3.7110106369704483</v>
+        <v>4.5606258125115007</v>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
@@ -24884,10 +24922,10 @@
         <v>6</v>
       </c>
       <c r="E8" s="20">
-        <v>329.36</v>
+        <v>286.55</v>
       </c>
       <c r="F8" s="39">
-        <v>0.2</v>
+        <v>0.35</v>
       </c>
       <c r="G8" s="30">
         <f>SUM(A3:A9)</f>
@@ -24895,11 +24933,11 @@
       </c>
       <c r="H8" s="49">
         <f>F8*B14/B13</f>
-        <v>7.718652841306789E-2</v>
+        <v>0.14386062902352806</v>
       </c>
       <c r="I8" s="45">
         <f>POWER((G8-E8*L1-M1)/H8,2)</f>
-        <v>2194.035653660856</v>
+        <v>8.598907696097316E-2</v>
       </c>
       <c r="J8" s="5">
         <v>7</v>
@@ -24909,12 +24947,12 @@
       </c>
       <c r="M8" s="20">
         <f>L2*B13</f>
-        <v>0.16018781854440389</v>
-      </c>
-      <c r="P8" s="18">
-        <v>336.85700000000003</v>
-      </c>
-      <c r="Q8" s="39">
+        <v>2.6570294182960381E-2</v>
+      </c>
+      <c r="P8" s="32">
+        <v>294.983</v>
+      </c>
+      <c r="Q8" s="47">
         <v>0.2</v>
       </c>
       <c r="R8" s="30">
@@ -24923,11 +24961,11 @@
       </c>
       <c r="S8" s="25">
         <f>Q8*B14/B13</f>
-        <v>7.718652841306789E-2</v>
+        <v>8.2206073727730311E-2</v>
       </c>
       <c r="T8" s="45">
         <f>POWER((R8-P8*W1-X1)/S8,2)</f>
-        <v>3284.7633362040519</v>
+        <v>1.0734113773240064</v>
       </c>
       <c r="U8" s="5">
         <v>7</v>
@@ -24937,7 +24975,7 @@
       </c>
       <c r="X8" s="20">
         <f>W2*B13</f>
-        <v>0.17463371392671176</v>
+        <v>9.3640847133686905E-3</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
@@ -24950,8 +24988,50 @@
       <c r="C9" s="5">
         <v>7</v>
       </c>
+      <c r="E9" s="20">
+        <v>329.36</v>
+      </c>
+      <c r="F9" s="39">
+        <v>0.35</v>
+      </c>
+      <c r="G9" s="30">
+        <f>SUM(A3:A10)</f>
+        <v>158.76000000000002</v>
+      </c>
+      <c r="H9" s="49">
+        <f>F9*B14/B13</f>
+        <v>0.14386062902352806</v>
+      </c>
+      <c r="I9" s="45">
+        <f>POWER((G9-E9*L1-M1)/H9,2)</f>
+        <v>19.662322431159701</v>
+      </c>
+      <c r="J9" s="5">
+        <v>8</v>
+      </c>
       <c r="M9" s="8" t="s">
         <v>54</v>
+      </c>
+      <c r="P9" s="18">
+        <v>336.85700000000003</v>
+      </c>
+      <c r="Q9" s="39">
+        <v>0.2</v>
+      </c>
+      <c r="R9" s="30">
+        <f>SUM(A3:A10)</f>
+        <v>158.76000000000002</v>
+      </c>
+      <c r="S9" s="25">
+        <f>Q9*B14/B13</f>
+        <v>8.2206073727730311E-2</v>
+      </c>
+      <c r="T9" s="45">
+        <f>POWER((R9-P9*W1-X1)/S9,2)</f>
+        <v>23.806835927896977</v>
+      </c>
+      <c r="U9" s="5">
+        <v>8</v>
       </c>
       <c r="X9" s="8" t="s">
         <v>55</v>
@@ -24982,15 +25062,15 @@
         <v>65</v>
       </c>
       <c r="M11" s="45">
-        <f>POWER((G2-L1*E2-M1)/H2,2)+POWER((G3-L1*E3-M1)/H3,2)+POWER((G4-L1*E4-M1)/H4,2)+POWER((G5-L1*E5-M1)/H5,2)+POWER((G6-L1*E6-M1)/H6,2)+POWER((G7-L1*E7-M1)/H7,2)+POWER((G8-L1*E8-M1)/H8,2)</f>
-        <v>11363.04118050017</v>
+        <f>SUM(I2:I9)</f>
+        <v>103.82683287832106</v>
       </c>
       <c r="W11" s="3" t="s">
         <v>65</v>
       </c>
       <c r="X11" s="45">
-        <f>POWER((R2-W1*P2-X1)/S2,2)+POWER((R3-W1*P3-X1)/S3,2)+POWER((R4-W1*P4-X1)/S4,2)+POWER((R5-W1*P5-X1)/S5,2)+POWER((R6-W1*P6-X1)/S6,2)+POWER((R7-W1*P7-X1)/S7,2)+POWER((R8-W1*P8-X1)/S8,2)</f>
-        <v>20208.098923970956</v>
+        <f>SUM(T2:T9)</f>
+        <v>61.879944732368791</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
@@ -25021,14 +25101,14 @@
       </c>
       <c r="M13" s="44">
         <f>M11/M12</f>
-        <v>2272.608236100034</v>
+        <v>20.76536657566421</v>
       </c>
       <c r="W13" s="3" t="s">
         <v>67</v>
       </c>
       <c r="X13" s="44">
         <f>X11/X12</f>
-        <v>4041.6197847941912</v>
+        <v>12.375988946473758</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
@@ -25036,7 +25116,7 @@
         <v>56</v>
       </c>
       <c r="B14" s="25">
-        <v>3.7846986256572199</v>
+        <v>4.0308227440028599</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>57</v>
@@ -25046,14 +25126,14 @@
       </c>
       <c r="M14" s="52">
         <f>_xlfn.CHISQ.DIST.RT(M11,M12)</f>
-        <v>0</v>
+        <v>8.2425201572806786E-21</v>
       </c>
       <c r="W14" s="51" t="s">
         <v>68</v>
       </c>
       <c r="X14" s="52">
         <f>_xlfn.CHISQ.DIST.RT(X11,X12)</f>
-        <v>0</v>
+        <v>4.9655157569106913E-12</v>
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
@@ -25084,7 +25164,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="G3:G8" formulaRange="1"/>
+    <ignoredError sqref="G3:G4" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -25094,7 +25174,7 @@
   <dimension ref="A1:Y18"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25676,14 +25756,14 @@
         <v>65</v>
       </c>
       <c r="M11" s="45">
-        <f>POWER((G2-L1*E2-M1)/H2,2)+POWER((G3-L1*E3-M1)/H3,2)+POWER((G4-L1*E4-M1)/H4,2)+POWER((G5-L1*E5-M1)/H5,2)+POWER((G6-L1*E6-M1)/H6,2)+POWER((G7-L1*E7-M1)/H7,2)+POWER((G8-L1*E8-M1)/H8,2)</f>
+        <f>SUM(I2:I8)</f>
         <v>42.302904238671431</v>
       </c>
       <c r="W11" s="3" t="s">
         <v>65</v>
       </c>
       <c r="X11" s="45">
-        <f>POWER((R2-W1*P2-X1)/S2,2)+POWER((R3-W1*P3-X1)/S3,2)+POWER((R4-W1*P4-X1)/S4,2)+POWER((R5-W1*P5-X1)/S5,2)+POWER((R6-W1*P6-X1)/S6,2)+POWER((R7-W1*P7-X1)/S7,2)+POWER((R8-W1*P8-X1)/S8,2)</f>
+        <f>SUM(T2:T8)</f>
         <v>20.505403217571835</v>
       </c>
     </row>
@@ -25778,7 +25858,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="G3:G8" formulaRange="1"/>
+    <ignoredError sqref="G3:G7" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -25787,8 +25867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF0B04D7-4CCB-4FB2-B94F-F6D78953706E}">
   <dimension ref="A1:Y21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="S15" sqref="S15"/>
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25849,10 +25929,10 @@
       <c r="Q1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="V1" s="58"/>
-      <c r="W1" s="58"/>
-      <c r="X1" s="58"/>
-      <c r="Y1" s="58"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="8"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
@@ -25885,11 +25965,11 @@
       </c>
       <c r="K2" s="4">
         <f>I2*B15*1000</f>
-        <v>0.39177463049525163</v>
+        <v>0.41725226955140982</v>
       </c>
       <c r="L2" s="45">
         <f>POWER((J2-H2*O1-P1)/K2,2)</f>
-        <v>13.661497775259402</v>
+        <v>12.04407690294326</v>
       </c>
       <c r="M2" s="5">
         <v>0</v>
@@ -25906,10 +25986,10 @@
       <c r="Q2" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="V2" s="59"/>
-      <c r="W2" s="59"/>
-      <c r="X2" s="60"/>
-      <c r="Y2" s="60"/>
+      <c r="V2" s="58"/>
+      <c r="W2" s="58"/>
+      <c r="X2" s="7"/>
+      <c r="Y2" s="7"/>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
@@ -25942,11 +26022,11 @@
       </c>
       <c r="K3" s="4">
         <f>I3*B15*1000</f>
-        <v>0.49987841857796617</v>
+        <v>0.53238619455211</v>
       </c>
       <c r="L3" s="45">
         <f>POWER((J3-H3*O1-P1)/K3,2)</f>
-        <v>1.8242690200694578</v>
+        <v>1.608288983449788</v>
       </c>
       <c r="M3" s="5">
         <v>1</v>
@@ -25957,10 +26037,10 @@
       <c r="P3" s="13">
         <v>1.3645886683994108</v>
       </c>
-      <c r="V3" s="59"/>
-      <c r="W3" s="59"/>
-      <c r="X3" s="60"/>
-      <c r="Y3" s="60"/>
+      <c r="V3" s="58"/>
+      <c r="W3" s="58"/>
+      <c r="X3" s="7"/>
+      <c r="Y3" s="7"/>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
@@ -25993,11 +26073,11 @@
       </c>
       <c r="K4" s="4">
         <f>I4*B15*1000</f>
-        <v>0.58909877201608751</v>
+        <v>0.62740866937436934</v>
       </c>
       <c r="L4" s="45">
         <f>POWER((J4-H4*O1-P1)/K4,2)</f>
-        <v>0.28023715448857101</v>
+        <v>0.24705913621233619</v>
       </c>
       <c r="M4" s="5">
         <v>2</v>
@@ -26008,10 +26088,10 @@
       <c r="P4" s="13">
         <v>7</v>
       </c>
-      <c r="V4" s="59"/>
-      <c r="W4" s="59"/>
-      <c r="X4" s="60"/>
-      <c r="Y4" s="60"/>
+      <c r="V4" s="58"/>
+      <c r="W4" s="58"/>
+      <c r="X4" s="7"/>
+      <c r="Y4" s="7"/>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
@@ -26044,11 +26124,11 @@
       </c>
       <c r="K5" s="4">
         <f>I5*B15*1000</f>
-        <v>0.66558397169773409</v>
+        <v>0.7088678060058482</v>
       </c>
       <c r="L5" s="45">
         <f>POWER((J5-H5*O1-P1)/K5,2)</f>
-        <v>2.5536094808151568</v>
+        <v>2.2512808970858815</v>
       </c>
       <c r="M5" s="5">
         <v>3</v>
@@ -26059,10 +26139,10 @@
       <c r="P5" s="13">
         <v>13.034715637468542</v>
       </c>
-      <c r="V5" s="59"/>
-      <c r="W5" s="59"/>
-      <c r="X5" s="60"/>
-      <c r="Y5" s="60"/>
+      <c r="V5" s="58"/>
+      <c r="W5" s="58"/>
+      <c r="X5" s="7"/>
+      <c r="Y5" s="7"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
@@ -26095,19 +26175,19 @@
       </c>
       <c r="K6" s="4">
         <f>I6*B15*1000</f>
-        <v>0.73234467402607828</v>
+        <v>0.77997004794564451</v>
       </c>
       <c r="L6" s="45">
         <f>POWER((J6-H6*O1-P1)/K6,2)</f>
-        <v>3.1583752490853101</v>
+        <v>2.7844468457349474</v>
       </c>
       <c r="M6" s="5">
         <v>4</v>
       </c>
-      <c r="V6" s="59"/>
-      <c r="W6" s="59"/>
-      <c r="X6" s="60"/>
-      <c r="Y6" s="60"/>
+      <c r="V6" s="58"/>
+      <c r="W6" s="58"/>
+      <c r="X6" s="7"/>
+      <c r="Y6" s="7"/>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
@@ -26140,11 +26220,11 @@
       </c>
       <c r="K7" s="4">
         <f>I7*B15*1000</f>
-        <v>0.79387610462793989</v>
+        <v>0.84550295147979271</v>
       </c>
       <c r="L7" s="45">
         <f>POWER((J7-H7*O1-P1)/K7,2)</f>
-        <v>4.0325971812595682</v>
+        <v>3.555167330015558</v>
       </c>
       <c r="M7" s="5">
         <v>5</v>
@@ -26153,22 +26233,22 @@
         <v>52</v>
       </c>
       <c r="P7" s="20">
-        <f>O1*0.0001</f>
-        <v>0.49633424327359427</v>
+        <f>O1*0.001</f>
+        <v>4.963342432735943</v>
       </c>
       <c r="R7" s="3" t="s">
         <v>65</v>
       </c>
       <c r="S7" s="45">
         <f>POWER((J2-H2*O1-P1)/K2,2)+POWER((J3-H3*O1-P1)/K3,2)+POWER((J4-H4*O1-P1)/K4,2)+POWER((J5-H5*O1-P1)/K5,2)+POWER((J6-H6*O1-P1)/K6,2)+POWER((J7-H7*O1-P1)/K7,2)+POWER((J8-H8*O1-P1)/K8,2)+POWER((J9-H9*O1-P1)/K9,2)+POWER((J10-H10*O1-P1)/K10,2)</f>
-        <v>31.17203852414368</v>
+        <v>27.481498396625668</v>
       </c>
       <c r="T7" s="53"/>
       <c r="U7" s="33"/>
-      <c r="V7" s="59"/>
-      <c r="W7" s="59"/>
-      <c r="X7" s="60"/>
-      <c r="Y7" s="60"/>
+      <c r="V7" s="58"/>
+      <c r="W7" s="58"/>
+      <c r="X7" s="7"/>
+      <c r="Y7" s="7"/>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
@@ -26201,11 +26281,11 @@
       </c>
       <c r="K8" s="4">
         <f>I8*B15*1000</f>
-        <v>0.84540841317396409</v>
+        <v>0.9003864764004107</v>
       </c>
       <c r="L8" s="45">
         <f>POWER((J8-H8*O1-P1)/K8,2)</f>
-        <v>0.13414177114650935</v>
+        <v>0.11826037189797788</v>
       </c>
       <c r="M8" s="5">
         <v>6</v>
@@ -26226,10 +26306,10 @@
       </c>
       <c r="T8" s="53"/>
       <c r="U8" s="54"/>
-      <c r="V8" s="59"/>
-      <c r="W8" s="59"/>
-      <c r="X8" s="60"/>
-      <c r="Y8" s="60"/>
+      <c r="V8" s="58"/>
+      <c r="W8" s="58"/>
+      <c r="X8" s="7"/>
+      <c r="Y8" s="7"/>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
@@ -26262,11 +26342,11 @@
       </c>
       <c r="K9" s="4">
         <f>I9*B15*1000</f>
-        <v>0.90071550562459723</v>
+        <v>0.95929026457613853</v>
       </c>
       <c r="L9" s="45">
         <f>POWER((J9-H9*O1-P1)/K9,2)</f>
-        <v>0.15285755120210137</v>
+        <v>0.13476034122757366</v>
       </c>
       <c r="M9" s="5">
         <v>7</v>
@@ -26276,14 +26356,14 @@
       </c>
       <c r="S9" s="44">
         <f>S7/S8</f>
-        <v>4.4531483605919542</v>
+        <v>3.9259283423750952</v>
       </c>
       <c r="T9" s="53"/>
       <c r="U9" s="53"/>
-      <c r="V9" s="59"/>
-      <c r="W9" s="59"/>
-      <c r="X9" s="60"/>
-      <c r="Y9" s="60"/>
+      <c r="V9" s="58"/>
+      <c r="W9" s="58"/>
+      <c r="X9" s="7"/>
+      <c r="Y9" s="7"/>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
@@ -26316,11 +26396,11 @@
       </c>
       <c r="K10" s="4">
         <f>I10*B15*1000</f>
-        <v>0.94486822648854818</v>
+        <v>1.0063142971534003</v>
       </c>
       <c r="L10" s="45">
         <f>POWER((J10-H10*O1-P1)/K10,2)</f>
-        <v>5.3744533408176016</v>
+        <v>4.7381575880583453</v>
       </c>
       <c r="M10" s="5">
         <v>8</v>
@@ -26330,14 +26410,14 @@
       </c>
       <c r="S10" s="52">
         <f>_xlfn.CHISQ.DIST.RT(S7,S8)</f>
-        <v>5.7791544522905257E-5</v>
+        <v>2.7290008748132445E-4</v>
       </c>
       <c r="T10" s="53"/>
       <c r="U10" s="56"/>
-      <c r="V10" s="59"/>
-      <c r="W10" s="59"/>
-      <c r="X10" s="60"/>
-      <c r="Y10" s="60"/>
+      <c r="V10" s="58"/>
+      <c r="W10" s="58"/>
+      <c r="X10" s="7"/>
+      <c r="Y10" s="7"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
@@ -26491,7 +26571,7 @@
         <v>56</v>
       </c>
       <c r="B15" s="25">
-        <v>3.7846986256572199</v>
+        <v>4.0308227440028599</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>63</v>

</xml_diff>

<commit_message>
Added data analysis for first part of 'oscillazioni' experiment
</commit_message>
<xml_diff>
--- a/oscillazioni/molla.xlsx
+++ b/oscillazioni/molla.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="1008" documentId="13_ncr:1_{19EF7A93-7410-479C-B5A9-9683ABBE8874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C39044F3-4487-43D3-9711-E27C90CE765D}"/>
+  <xr:revisionPtr revIDLastSave="1299" documentId="13_ncr:1_{19EF7A93-7410-479C-B5A9-9683ABBE8874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{42AD59CF-24CD-40BD-8C4C-B5825BF3E232}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Statico - Calibro" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="74">
   <si>
     <t>m [g]</t>
   </si>
@@ -348,29 +348,6 @@
     <t>h4 [mm]</t>
   </si>
   <si>
-    <r>
-      <t>Δh</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>[mm]</t>
-    </r>
-  </si>
-  <si>
     <t>h5 [mm]</t>
   </si>
   <si>
@@ -402,29 +379,6 @@
   </si>
   <si>
     <t>σh4 [mm]</t>
-  </si>
-  <si>
-    <r>
-      <t>σ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Δh </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>[mm]</t>
-    </r>
   </si>
   <si>
     <t>σh5 [mm]</t>
@@ -712,18 +666,107 @@
       <t>contributo</t>
     </r>
   </si>
+  <si>
+    <r>
+      <t>h</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[mm]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>σ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Δh </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>[mm]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Δh</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>[mm]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>σ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Δh </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>[mm]</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.000000%"/>
-    <numFmt numFmtId="168" formatCode="0.00000000000000"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -790,18 +833,6 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -816,6 +847,34 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -832,7 +891,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -970,11 +1029,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1037,17 +1118,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1074,10 +1144,10 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="8" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="10" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1085,12 +1155,11 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1100,13 +1169,39 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1387,17 +1482,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M19"/>
+  <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="4.5703125" customWidth="1"/>
     <col min="12" max="12" width="9.140625" customWidth="1"/>
-    <col min="13" max="13" width="35.42578125" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -1410,8 +1505,8 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
+      <c r="E1" s="65" t="s">
+        <v>70</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>4</v>
@@ -1425,8 +1520,8 @@
       <c r="I1" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="16" t="s">
-        <v>8</v>
+      <c r="J1" s="73" t="s">
+        <v>72</v>
       </c>
       <c r="K1" s="16" t="s">
         <v>9</v>
@@ -1458,25 +1553,25 @@
         <v>341.81</v>
       </c>
       <c r="H2" s="6">
-        <f t="shared" ref="H2:H9" si="0">AVERAGE(E2,F2,G2)</f>
+        <f t="shared" ref="H2:H6" si="0">AVERAGE(E2,F2,G2)</f>
         <v>341.59</v>
       </c>
       <c r="I2" s="14">
-        <f t="shared" ref="I2:I9" si="1">_xlfn.STDEV.S(E2,F2,G2)/SQRT(3)</f>
+        <f t="shared" ref="I2:I6" si="1">_xlfn.STDEV.S(E2,F2,G2)/SQRT(3)</f>
         <v>0.3251666239535273</v>
       </c>
-      <c r="J2" s="17" t="s">
+      <c r="J2" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="17" t="s">
+      <c r="K2" s="71" t="s">
         <v>12</v>
       </c>
       <c r="L2" s="5">
         <v>0</v>
       </c>
-      <c r="M2" s="59">
-        <f>B14*SUM(A4:A9)/(H3-H9)</f>
-        <v>4.0308227440028572</v>
+      <c r="M2" s="25">
+        <f>B14*SUM(A5:A9)/(H4-H9)</f>
+        <v>4.7473667850461219</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -1509,11 +1604,11 @@
         <f t="shared" si="1"/>
         <v>0.54049360156557669</v>
       </c>
-      <c r="J3" s="18">
+      <c r="J3" s="6">
         <f>H2-H3</f>
         <v>39.579999999999984</v>
       </c>
-      <c r="K3" s="18">
+      <c r="K3" s="6">
         <f>SQRT(POWER(I2,2)+POWER(I3,2))</f>
         <v>0.63076672920079024</v>
       </c>
@@ -1551,11 +1646,11 @@
         <f t="shared" si="1"/>
         <v>0.45999999999999852</v>
       </c>
-      <c r="J4" s="18">
+      <c r="J4" s="6">
         <f>H2-H4</f>
         <v>81.319999999999993</v>
       </c>
-      <c r="K4" s="18">
+      <c r="K4" s="6">
         <f>SQRT(POWER(I2,2)+POWER(I4,2))</f>
         <v>0.56332347131406957</v>
       </c>
@@ -1573,33 +1668,33 @@
       <c r="C5" s="5">
         <v>3</v>
       </c>
-      <c r="E5" s="6">
-        <f>37.26+179.81</f>
-        <v>217.07</v>
-      </c>
-      <c r="F5" s="6">
-        <f>39+179.81</f>
-        <v>218.81</v>
-      </c>
-      <c r="G5" s="6">
+      <c r="E5" s="61">
+        <f>37.06+179.81</f>
+        <v>216.87</v>
+      </c>
+      <c r="F5" s="61">
+        <f>39.2+179.81</f>
+        <v>219.01</v>
+      </c>
+      <c r="G5" s="61">
         <f>38.64+179.81</f>
         <v>218.45</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="61">
         <f t="shared" si="0"/>
         <v>218.10999999999999</v>
       </c>
-      <c r="I5" s="14">
+      <c r="I5" s="62">
         <f t="shared" si="1"/>
-        <v>0.53028294334251558</v>
-      </c>
-      <c r="J5" s="18">
+        <v>0.64072875176109234</v>
+      </c>
+      <c r="J5" s="6">
         <f>H2-H5</f>
         <v>123.47999999999999</v>
       </c>
-      <c r="K5" s="18">
+      <c r="K5" s="6">
         <f>SQRT(POWER(I2,2)+POWER(I5,2))</f>
-        <v>0.62203965575623565</v>
+        <v>0.71851699121639578</v>
       </c>
       <c r="L5" s="5">
         <v>3</v>
@@ -1615,30 +1710,30 @@
       <c r="C6" s="5">
         <v>4</v>
       </c>
-      <c r="E6" s="6">
-        <v>139</v>
-      </c>
-      <c r="F6" s="6">
-        <v>139.19999999999999</v>
-      </c>
-      <c r="G6" s="6">
-        <v>138.84</v>
+      <c r="E6" s="40">
+        <v>178.31</v>
+      </c>
+      <c r="F6" s="40">
+        <v>179.35</v>
+      </c>
+      <c r="G6" s="40">
+        <v>180.39</v>
       </c>
       <c r="H6" s="6">
         <f t="shared" si="0"/>
-        <v>139.01333333333332</v>
+        <v>179.35</v>
       </c>
       <c r="I6" s="14">
         <f t="shared" si="1"/>
-        <v>0.10413666234541774</v>
-      </c>
-      <c r="J6" s="18">
+        <v>0.60044427995720628</v>
+      </c>
+      <c r="J6" s="6">
         <f>H2-H6</f>
-        <v>202.57666666666665</v>
-      </c>
-      <c r="K6" s="39">
+        <v>162.23999999999998</v>
+      </c>
+      <c r="K6" s="6">
         <f>SQRT(POWER(I2,2)+POWER(I6,2))</f>
-        <v>0.34143488072805067</v>
+        <v>0.68283721827875099</v>
       </c>
       <c r="L6" s="5">
         <v>4</v>
@@ -1654,30 +1749,30 @@
       <c r="C7" s="5">
         <v>5</v>
       </c>
-      <c r="E7" s="6">
-        <v>97.4</v>
-      </c>
-      <c r="F7" s="6">
-        <v>97</v>
-      </c>
-      <c r="G7" s="6">
-        <v>97.3</v>
-      </c>
-      <c r="H7" s="6">
-        <f t="shared" si="0"/>
-        <v>97.233333333333334</v>
-      </c>
-      <c r="I7" s="14">
-        <f t="shared" si="1"/>
-        <v>0.12018504251546737</v>
-      </c>
-      <c r="J7" s="18">
+      <c r="E7" s="63">
+        <v>139</v>
+      </c>
+      <c r="F7" s="63">
+        <v>140.1</v>
+      </c>
+      <c r="G7" s="63">
+        <v>137.94</v>
+      </c>
+      <c r="H7" s="63">
+        <f>AVERAGE(E7,F7,G7)</f>
+        <v>139.01333333333335</v>
+      </c>
+      <c r="I7" s="64">
+        <f>_xlfn.STDEV.S(E7,F7,G7)/SQRT(3)</f>
+        <v>0.62357392861187144</v>
+      </c>
+      <c r="J7" s="6">
         <f>H2-H7</f>
-        <v>244.35666666666663</v>
-      </c>
-      <c r="K7" s="39">
+        <v>202.57666666666663</v>
+      </c>
+      <c r="K7" s="72">
         <f>SQRT(POWER(I2,2)+POWER(I7,2))</f>
-        <v>0.3466666666666689</v>
+        <v>0.70326223969283175</v>
       </c>
       <c r="L7" s="5">
         <v>5</v>
@@ -1694,35 +1789,32 @@
         <v>6</v>
       </c>
       <c r="E8" s="6">
-        <v>55.4</v>
+        <v>98.4</v>
       </c>
       <c r="F8" s="6">
-        <v>55.6</v>
+        <v>96</v>
       </c>
       <c r="G8" s="6">
-        <v>55.12</v>
+        <v>97.3</v>
       </c>
       <c r="H8" s="6">
-        <f t="shared" si="0"/>
-        <v>55.373333333333335</v>
+        <f>AVERAGE(E8,F8,G8)</f>
+        <v>97.233333333333334</v>
       </c>
       <c r="I8" s="14">
-        <f t="shared" si="1"/>
-        <v>0.13920408678547513</v>
-      </c>
-      <c r="J8" s="18">
+        <f>_xlfn.STDEV.S(E8,F8,G8)/SQRT(3)</f>
+        <v>0.6936217348894953</v>
+      </c>
+      <c r="J8" s="6">
         <f>H2-H8</f>
-        <v>286.21666666666664</v>
-      </c>
-      <c r="K8" s="39">
+        <v>244.35666666666663</v>
+      </c>
+      <c r="K8" s="72">
         <f>SQRT(POWER(I2,2)+POWER(I8,2))</f>
-        <v>0.35371049053019721</v>
+        <v>0.76605772918524095</v>
       </c>
       <c r="L8" s="5">
         <v>6</v>
-      </c>
-      <c r="M8" s="33" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -1736,35 +1828,35 @@
         <v>7</v>
       </c>
       <c r="E9" s="6">
-        <v>12.5</v>
+        <v>54.9</v>
       </c>
       <c r="F9" s="6">
-        <v>12.8</v>
+        <v>56.1</v>
       </c>
       <c r="G9" s="6">
-        <v>12.4</v>
+        <v>55.12</v>
       </c>
       <c r="H9" s="6">
-        <f t="shared" si="0"/>
-        <v>12.566666666666668</v>
+        <f>AVERAGE(E9,F9,G9)</f>
+        <v>55.373333333333335</v>
       </c>
       <c r="I9" s="14">
-        <f t="shared" si="1"/>
-        <v>0.12018504251546647</v>
-      </c>
-      <c r="J9" s="18">
+        <f>_xlfn.STDEV.S(E9,F9,G9)/SQRT(3)</f>
+        <v>0.36884203182994924</v>
+      </c>
+      <c r="J9" s="6">
         <f>H2-H9</f>
-        <v>329.02333333333331</v>
-      </c>
-      <c r="K9" s="39">
+        <v>286.21666666666664</v>
+      </c>
+      <c r="K9" s="72">
         <f>SQRT(POWER(I2,2)+POWER(I9,2))</f>
-        <v>0.34666666666666862</v>
+        <v>0.49170903772228952</v>
       </c>
       <c r="L9" s="5">
         <v>7</v>
       </c>
       <c r="M9" s="33" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -1778,10 +1870,37 @@
         <v>8</v>
       </c>
       <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
+      <c r="E10" s="6">
+        <v>11.5</v>
+      </c>
+      <c r="F10" s="6">
+        <v>13.7</v>
+      </c>
+      <c r="G10" s="6">
+        <v>12.5</v>
+      </c>
+      <c r="H10" s="6">
+        <f>AVERAGE(E10,F10,G10)</f>
+        <v>12.566666666666668</v>
+      </c>
+      <c r="I10" s="14">
+        <f>_xlfn.STDEV.S(E10,F10,G10)/SQRT(3)</f>
+        <v>0.63595946761129696</v>
+      </c>
+      <c r="J10" s="6">
+        <f>H2-H10</f>
+        <v>329.02333333333331</v>
+      </c>
+      <c r="K10" s="72">
+        <f>SQRT(POWER(I2,2)+POWER(I10,2))</f>
+        <v>0.71426730134997707</v>
+      </c>
+      <c r="L10" s="5">
+        <v>8</v>
+      </c>
+      <c r="M10" s="33" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
@@ -1796,33 +1915,11 @@
       <c r="D11" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I11" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="J11" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="K11" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M11" s="24" t="s">
-        <v>10</v>
-      </c>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="K11" s="68"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
@@ -1834,65 +1931,64 @@
       <c r="C12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="6">
-        <v>28.64</v>
-      </c>
-      <c r="F12" s="6">
-        <v>27.8</v>
-      </c>
-      <c r="G12" s="6">
-        <v>28.58</v>
-      </c>
-      <c r="H12" s="6">
-        <f t="shared" ref="H12:H19" si="2">AVERAGE(E12,F12,G12)</f>
-        <v>28.34</v>
-      </c>
-      <c r="I12" s="14">
-        <f t="shared" ref="I12:I19" si="3">_xlfn.STDEV.S(E12,F12,G12)/SQRT(3)</f>
-        <v>0.27055498516937326</v>
-      </c>
-      <c r="J12" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="K12" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="L12" s="5">
-        <v>1</v>
-      </c>
-      <c r="M12" s="25">
-        <f>B14*SUM(A5:A8)/(H17-H13)</f>
-        <v>7.7240619386808094</v>
+      <c r="E12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J12" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="K12" s="69" t="s">
+        <v>71</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M12" s="24" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E13" s="6">
-        <v>53.34</v>
+        <v>28.64</v>
       </c>
       <c r="F13" s="6">
-        <v>53</v>
+        <v>27.8</v>
       </c>
       <c r="G13" s="6">
-        <v>53.3</v>
+        <v>28.58</v>
       </c>
       <c r="H13" s="6">
-        <f t="shared" si="2"/>
-        <v>53.213333333333331</v>
+        <f t="shared" ref="H13:H20" si="2">AVERAGE(E13,F13,G13)</f>
+        <v>28.34</v>
       </c>
       <c r="I13" s="14">
-        <f t="shared" si="3"/>
-        <v>0.10728984626287418</v>
-      </c>
-      <c r="J13" s="18">
-        <f>H13-H12</f>
-        <v>24.873333333333331</v>
-      </c>
-      <c r="K13" s="39">
-        <f>SQRT(POWER(I12,2)+POWER(I13,2))</f>
-        <v>0.2910517327059074</v>
+        <f t="shared" ref="I13:I20" si="3">_xlfn.STDEV.S(E13,F13,G13)/SQRT(3)</f>
+        <v>0.27055498516937326</v>
+      </c>
+      <c r="J13" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="K13" s="70" t="s">
+        <v>12</v>
       </c>
       <c r="L13" s="5">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="M13" s="25">
+        <f>B14*SUM(A5:A8)/(H18-H14)</f>
+        <v>7.7240619386808094</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -1903,181 +1999,211 @@
         <v>9.8066300000000002</v>
       </c>
       <c r="E14" s="6">
-        <v>79.599999999999994</v>
+        <v>53.34</v>
       </c>
       <c r="F14" s="6">
-        <v>78.5</v>
+        <v>53</v>
       </c>
       <c r="G14" s="6">
-        <v>78.400000000000006</v>
+        <v>53.3</v>
       </c>
       <c r="H14" s="6">
         <f t="shared" si="2"/>
-        <v>78.833333333333329</v>
+        <v>53.213333333333331</v>
       </c>
       <c r="I14" s="14">
         <f t="shared" si="3"/>
-        <v>0.3844187531556903</v>
+        <v>0.10728984626287418</v>
       </c>
       <c r="J14" s="18">
-        <f>H14-H12</f>
-        <v>50.493333333333325</v>
-      </c>
-      <c r="K14" s="18">
-        <f>SQRT(POWER(I12,2)+POWER(I14,2))</f>
-        <v>0.47008273503477588</v>
+        <f>H14-H13</f>
+        <v>24.873333333333331</v>
+      </c>
+      <c r="K14" s="67">
+        <f>SQRT(POWER(I13,2)+POWER(I14,2))</f>
+        <v>0.2910517327059074</v>
       </c>
       <c r="L14" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E15" s="6">
-        <v>103</v>
+        <v>79.599999999999994</v>
       </c>
       <c r="F15" s="6">
-        <v>103.9</v>
+        <v>78.5</v>
       </c>
       <c r="G15" s="6">
-        <v>103.5</v>
+        <v>78.400000000000006</v>
       </c>
       <c r="H15" s="6">
         <f t="shared" si="2"/>
-        <v>103.46666666666665</v>
+        <v>78.833333333333329</v>
       </c>
       <c r="I15" s="14">
         <f t="shared" si="3"/>
-        <v>0.26034165586355673</v>
+        <v>0.3844187531556903</v>
       </c>
       <c r="J15" s="18">
-        <f>H15-H12</f>
-        <v>75.126666666666651</v>
-      </c>
-      <c r="K15" s="18">
-        <f>SQRT(POWER(I12,2)+POWER(I15,2))</f>
-        <v>0.37547007574210012</v>
+        <f>H15-H13</f>
+        <v>50.493333333333325</v>
+      </c>
+      <c r="K15" s="67">
+        <f>SQRT(POWER(I13,2)+POWER(I15,2))</f>
+        <v>0.47008273503477588</v>
       </c>
       <c r="L15" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E16" s="6">
-        <v>130</v>
+        <v>103</v>
       </c>
       <c r="F16" s="6">
-        <v>131.30000000000001</v>
+        <v>103.9</v>
       </c>
       <c r="G16" s="6">
-        <v>130.19999999999999</v>
+        <v>103.5</v>
       </c>
       <c r="H16" s="6">
         <f t="shared" si="2"/>
-        <v>130.5</v>
+        <v>103.46666666666665</v>
       </c>
       <c r="I16" s="14">
         <f t="shared" si="3"/>
-        <v>0.40414518843274322</v>
+        <v>0.26034165586355673</v>
       </c>
       <c r="J16" s="18">
-        <f>H16-H12</f>
-        <v>102.16</v>
-      </c>
-      <c r="K16" s="18">
-        <f>SQRT(POWER(I12,2)+POWER(I16,2))</f>
-        <v>0.48634692692905679</v>
+        <f>H16-H13</f>
+        <v>75.126666666666651</v>
+      </c>
+      <c r="K16" s="67">
+        <f>SQRT(POWER(I13,2)+POWER(I16,2))</f>
+        <v>0.37547007574210012</v>
       </c>
       <c r="L16" s="5">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E17" s="6">
-        <v>153.80000000000001</v>
+        <v>130</v>
       </c>
       <c r="F17" s="6">
-        <v>153.9</v>
+        <v>131.30000000000001</v>
       </c>
       <c r="G17" s="6">
-        <v>153.63999999999999</v>
+        <v>130.19999999999999</v>
       </c>
       <c r="H17" s="6">
         <f t="shared" si="2"/>
-        <v>153.78</v>
+        <v>130.5</v>
       </c>
       <c r="I17" s="14">
         <f t="shared" si="3"/>
-        <v>7.5718777944009857E-2</v>
+        <v>0.40414518843274322</v>
       </c>
       <c r="J17" s="18">
-        <f>H17-H12</f>
-        <v>125.44</v>
-      </c>
-      <c r="K17" s="39">
-        <f>SQRT(POWER(I12,2)+POWER(I17,2))</f>
-        <v>0.280950766742741</v>
+        <f>H17-H13</f>
+        <v>102.16</v>
+      </c>
+      <c r="K17" s="67">
+        <f>SQRT(POWER(I13,2)+POWER(I17,2))</f>
+        <v>0.48634692692905679</v>
       </c>
       <c r="L17" s="5">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E18" s="6">
-        <v>179.7</v>
+        <v>153.80000000000001</v>
       </c>
       <c r="F18" s="6">
-        <v>179.98</v>
+        <v>153.9</v>
       </c>
       <c r="G18" s="6">
-        <v>179.8</v>
+        <v>153.63999999999999</v>
       </c>
       <c r="H18" s="6">
         <f t="shared" si="2"/>
-        <v>179.82666666666668</v>
+        <v>153.78</v>
       </c>
       <c r="I18" s="14">
         <f t="shared" si="3"/>
-        <v>8.1921371516295832E-2</v>
+        <v>7.5718777944009857E-2</v>
       </c>
       <c r="J18" s="18">
-        <f>H18-H12</f>
-        <v>151.48666666666668</v>
-      </c>
-      <c r="K18" s="39">
-        <f>SQRT(POWER(I12,2)+POWER(I18,2))</f>
-        <v>0.28268553396152191</v>
+        <f>H18-H13</f>
+        <v>125.44</v>
+      </c>
+      <c r="K18" s="67">
+        <f>SQRT(POWER(I13,2)+POWER(I18,2))</f>
+        <v>0.280950766742741</v>
       </c>
       <c r="L18" s="5">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E19" s="6">
-        <v>206.5</v>
+        <v>179.7</v>
       </c>
       <c r="F19" s="6">
-        <v>206.5</v>
+        <v>179.98</v>
       </c>
       <c r="G19" s="6">
-        <v>206.18</v>
+        <v>179.8</v>
       </c>
       <c r="H19" s="6">
         <f t="shared" si="2"/>
-        <v>206.39333333333335</v>
+        <v>179.82666666666668</v>
       </c>
       <c r="I19" s="14">
         <f t="shared" si="3"/>
+        <v>8.1921371516295832E-2</v>
+      </c>
+      <c r="J19" s="18">
+        <f>H19-H13</f>
+        <v>151.48666666666668</v>
+      </c>
+      <c r="K19" s="67">
+        <f>SQRT(POWER(I13,2)+POWER(I19,2))</f>
+        <v>0.28268553396152191</v>
+      </c>
+      <c r="L19" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E20" s="6">
+        <v>206.5</v>
+      </c>
+      <c r="F20" s="6">
+        <v>206.5</v>
+      </c>
+      <c r="G20" s="6">
+        <v>206.18</v>
+      </c>
+      <c r="H20" s="6">
+        <f t="shared" si="2"/>
+        <v>206.39333333333335</v>
+      </c>
+      <c r="I20" s="14">
+        <f t="shared" si="3"/>
         <v>0.1066666666666644</v>
       </c>
-      <c r="J19" s="18">
-        <f>H19-H12</f>
+      <c r="J20" s="18">
+        <f>H20-H13</f>
         <v>178.05333333333334</v>
       </c>
-      <c r="K19" s="39">
-        <f>SQRT(POWER(I12,2)+POWER(I19,2))</f>
+      <c r="K20" s="67">
+        <f>SQRT(POWER(I13,2)+POWER(I20,2))</f>
         <v>0.29082258814916195</v>
       </c>
-      <c r="L19" s="5">
+      <c r="L20" s="5">
         <v>8</v>
       </c>
     </row>
@@ -2091,8 +2217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2D4EB93-7770-4A45-A697-00620671C631}">
   <dimension ref="A1:AE381"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="AB4" sqref="AB4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2105,6 +2231,7 @@
     <col min="16" max="16" width="13.85546875" customWidth="1"/>
     <col min="19" max="19" width="13.85546875" customWidth="1"/>
     <col min="22" max="22" width="13.7109375" customWidth="1"/>
+    <col min="24" max="24" width="9.140625" customWidth="1"/>
     <col min="26" max="26" width="13.85546875" customWidth="1"/>
     <col min="29" max="29" width="13.7109375" customWidth="1"/>
   </cols>
@@ -2143,20 +2270,20 @@
       <c r="L1" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="33" t="s">
+      <c r="M1" s="74" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="34" t="s">
+      <c r="N1" s="75" t="s">
         <v>24</v>
       </c>
-      <c r="O1" s="35" t="s">
-        <v>25</v>
+      <c r="O1" s="73" t="s">
+        <v>72</v>
       </c>
       <c r="P1" t="s">
         <v>19</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="R1" s="16" t="s">
         <v>8</v>
@@ -2165,16 +2292,16 @@
         <v>19</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="V1" t="s">
         <v>19</v>
       </c>
       <c r="W1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="X1" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="Y1" s="16" t="s">
         <v>8</v>
@@ -2183,7 +2310,7 @@
         <v>19</v>
       </c>
       <c r="AA1" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AB1" s="16" t="s">
         <v>8</v>
@@ -2192,7 +2319,7 @@
         <v>19</v>
       </c>
       <c r="AD1" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AE1" s="16" t="s">
         <v>8</v>
@@ -2239,14 +2366,14 @@
         <f>B2-K2</f>
         <v>124.0196503641456</v>
       </c>
-      <c r="M2" s="33">
+      <c r="M2" s="74">
         <v>0.26332699999999998</v>
       </c>
-      <c r="N2" s="36">
+      <c r="N2" s="76">
         <f>1000*AVERAGE(M2:M365)+X2</f>
         <v>396.65741609785618</v>
       </c>
-      <c r="O2" s="37">
+      <c r="O2" s="77">
         <f>B2-N2</f>
         <v>166.95291561168074</v>
       </c>
@@ -2311,13 +2438,13 @@
         <v>0.43103200000000003</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D3">
         <v>0.39146399999999998</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F3" s="16" t="s">
         <v>9</v>
@@ -2326,7 +2453,7 @@
         <v>0.35123100000000002</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I3" s="16" t="s">
         <v>9</v>
@@ -2335,25 +2462,25 @@
         <v>0.30608000000000002</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L3" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="M3" s="33">
+      <c r="M3" s="74">
         <v>0.26349299999999998</v>
       </c>
-      <c r="N3" s="34" t="s">
-        <v>36</v>
-      </c>
-      <c r="O3" s="35" t="s">
-        <v>37</v>
+      <c r="N3" s="75" t="s">
+        <v>35</v>
+      </c>
+      <c r="O3" s="73" t="s">
+        <v>73</v>
       </c>
       <c r="P3">
         <v>0.22136800000000001</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="R3" s="16" t="s">
         <v>9</v>
@@ -2362,13 +2489,13 @@
         <v>0.176121</v>
       </c>
       <c r="T3" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="V3">
         <v>0.313803</v>
       </c>
       <c r="W3" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="Y3" s="16" t="s">
         <v>9</v>
@@ -2377,7 +2504,7 @@
         <v>0.26866899999999999</v>
       </c>
       <c r="AA3" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="AB3" s="16" t="s">
         <v>9</v>
@@ -2386,7 +2513,7 @@
         <v>0.22773699999999999</v>
       </c>
       <c r="AD3" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="AE3" s="16" t="s">
         <v>9</v>
@@ -2433,14 +2560,14 @@
         <f>SQRT(POWER(B4,2)+POWER(K4,2))</f>
         <v>6.2058360081640472E-2</v>
       </c>
-      <c r="M4" s="33">
+      <c r="M4" s="74">
         <v>0.26384299999999999</v>
       </c>
-      <c r="N4" s="38">
+      <c r="N4" s="78">
         <f>1000*_xlfn.STDEV.S(M2:M365)/SQRT(365-1)</f>
         <v>4.4972905737269232E-2</v>
       </c>
-      <c r="O4" s="39">
+      <c r="O4" s="79">
         <f>SQRT(POWER(B4,2)+POWER(N4,2))</f>
         <v>4.8014315615057333E-2</v>
       </c>
@@ -2509,11 +2636,11 @@
       <c r="J5">
         <v>0.308396</v>
       </c>
-      <c r="M5" s="33">
+      <c r="M5" s="74">
         <v>0.264015</v>
       </c>
-      <c r="N5" s="33"/>
-      <c r="O5" s="33"/>
+      <c r="N5" s="74"/>
+      <c r="O5" s="74"/>
       <c r="P5">
         <v>0.221192</v>
       </c>
@@ -2543,12 +2670,12 @@
       <c r="J6">
         <v>0.308396</v>
       </c>
-      <c r="M6" s="33">
+      <c r="M6" s="74">
         <v>0.26419199999999998</v>
       </c>
-      <c r="N6" s="33"/>
-      <c r="O6" s="33" t="s">
-        <v>43</v>
+      <c r="N6" s="74"/>
+      <c r="O6" s="74" t="s">
+        <v>41</v>
       </c>
       <c r="P6">
         <v>0.221192</v>
@@ -2603,7 +2730,7 @@
         <v>0.430697</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D8">
         <v>0.392488</v>
@@ -14030,7 +14157,7 @@
   <dimension ref="A1:AD454"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14083,7 +14210,7 @@
         <v>19</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="R1" s="16" t="s">
         <v>8</v>
@@ -14092,7 +14219,7 @@
         <v>19</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="V1" s="16" t="s">
         <v>8</v>
@@ -14101,7 +14228,7 @@
         <v>19</v>
       </c>
       <c r="Y1" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Z1" s="16" t="s">
         <v>8</v>
@@ -14110,7 +14237,7 @@
         <v>19</v>
       </c>
       <c r="AC1" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AD1" s="16" t="s">
         <v>8</v>
@@ -14207,13 +14334,13 @@
         <v>0.58544099999999999</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D3">
         <v>0.55865600000000004</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F3" s="16" t="s">
         <v>9</v>
@@ -14222,7 +14349,7 @@
         <v>0.53332900000000005</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="J3" s="16" t="s">
         <v>9</v>
@@ -14231,7 +14358,7 @@
         <v>0.50705599999999995</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N3" s="16" t="s">
         <v>9</v>
@@ -14240,7 +14367,7 @@
         <v>0.48296600000000001</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="R3" s="16" t="s">
         <v>9</v>
@@ -14249,7 +14376,7 @@
         <v>0.45957500000000001</v>
       </c>
       <c r="U3" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="V3" s="16" t="s">
         <v>9</v>
@@ -14258,7 +14385,7 @@
         <v>0.43360300000000002</v>
       </c>
       <c r="Y3" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="Z3" s="16" t="s">
         <v>9</v>
@@ -14267,7 +14394,7 @@
         <v>0.41075200000000001</v>
       </c>
       <c r="AC3" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="AD3" s="16" t="s">
         <v>9</v>
@@ -24436,8 +24563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B459E249-CE69-4C2B-8F77-71C2DA9D2D63}">
   <dimension ref="A1:Y18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="M1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24460,7 +24587,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E1" s="16" t="s">
         <v>8</v>
@@ -24469,26 +24596,26 @@
         <v>9</v>
       </c>
       <c r="G1" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="K1" s="21" t="s">
         <v>46</v>
-      </c>
-      <c r="H1" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="I1" s="48" t="s">
-        <v>71</v>
-      </c>
-      <c r="K1" s="21" t="s">
-        <v>48</v>
       </c>
       <c r="L1" s="13" cm="1">
         <f t="array" ref="L1:M5">LINEST(G2:G9,E2:E9,TRUE,TRUE)</f>
-        <v>0.48213257339934595</v>
+        <v>0.48252067444082619</v>
       </c>
       <c r="M1" s="13">
-        <v>0.60272555380251447</v>
+        <v>0.55075574808584804</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="P1" s="16" t="s">
         <v>8</v>
@@ -24497,26 +24624,26 @@
         <v>9</v>
       </c>
       <c r="R1" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="S1" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="T1" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="V1" s="21" t="s">
         <v>46</v>
-      </c>
-      <c r="S1" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="T1" s="48" t="s">
-        <v>71</v>
-      </c>
-      <c r="V1" s="21" t="s">
-        <v>48</v>
       </c>
       <c r="W1" s="13" cm="1">
         <f t="array" ref="W1:X5">LINEST(R2:R9,P2:P9,TRUE,TRUE)</f>
-        <v>0.4650553566833357</v>
+        <v>0.46506362782995114</v>
       </c>
       <c r="X1" s="13">
-        <v>1.7017457893045247</v>
+        <v>1.6964405852504001</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
@@ -24530,42 +24657,42 @@
         <v>11</v>
       </c>
       <c r="E2" s="19">
-        <v>39.909999999999997</v>
+        <v>39.58</v>
       </c>
       <c r="F2" s="18">
-        <v>0.54</v>
+        <v>0.63</v>
       </c>
       <c r="G2" s="30">
         <f>SUM(A3:A3)</f>
         <v>19.829999999999998</v>
       </c>
-      <c r="H2" s="49">
+      <c r="H2" s="44">
         <f>F2*B14/B13</f>
-        <v>0.22195639906487186</v>
-      </c>
-      <c r="I2" s="45">
+        <v>0.30498153540809181</v>
+      </c>
+      <c r="I2" s="40">
         <f>POWER((G2-E2*L1-M1)/H2,2)</f>
-        <v>4.3485311504757812E-3</v>
+        <v>0.35251247267364477</v>
       </c>
       <c r="J2" s="5">
         <v>1</v>
       </c>
       <c r="K2" s="21" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L2" s="13">
-        <v>2.7094215018778501E-3</v>
+        <v>1.8598656333942596E-3</v>
       </c>
       <c r="M2" s="13">
-        <v>0.55929892346831012</v>
+        <v>0.38380071308332225</v>
       </c>
       <c r="N2" s="23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="P2" s="20">
         <v>38.890999999999998</v>
       </c>
-      <c r="Q2" s="39">
+      <c r="Q2" s="34">
         <v>0.2</v>
       </c>
       <c r="R2" s="30">
@@ -24574,26 +24701,26 @@
       </c>
       <c r="S2" s="25">
         <f>Q2*B14/B13</f>
-        <v>8.2206073727730311E-2</v>
-      </c>
-      <c r="T2" s="45">
+        <v>9.6819535050187894E-2</v>
+      </c>
+      <c r="T2" s="40">
         <f>POWER((R2-P2*W1-X1)/S2,2)</f>
-        <v>0.25838109151036698</v>
+        <v>0.23334916102109501</v>
       </c>
       <c r="U2" s="5">
         <v>1</v>
       </c>
       <c r="V2" s="21" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="W2" s="13">
-        <v>9.5487284759073106E-4</v>
+        <v>9.7165723987595548E-4</v>
       </c>
       <c r="X2" s="13">
-        <v>0.20235481781272108</v>
+        <v>0.20591173395243895</v>
       </c>
       <c r="Y2" s="23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -24607,36 +24734,36 @@
         <v>1</v>
       </c>
       <c r="E3" s="20">
-        <v>81.650000000000006</v>
+        <v>81.319999999999993</v>
       </c>
       <c r="F3" s="18">
-        <v>0.46</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="G3" s="30">
         <f>SUM(A3:A4)</f>
         <v>39.61</v>
       </c>
-      <c r="H3" s="50">
+      <c r="H3" s="45">
         <f>F3*B14/B13</f>
-        <v>0.18907396957377973</v>
-      </c>
-      <c r="I3" s="45">
+        <v>0.27109469814052611</v>
+      </c>
+      <c r="I3" s="40">
         <f>POWER((G3-E3*L1-M1)/H3,2)</f>
-        <v>3.6021586176783518</v>
+        <v>0.43762056438873709</v>
       </c>
       <c r="J3" s="5">
         <v>2</v>
       </c>
       <c r="L3" s="13">
-        <v>0.99981055237513417</v>
+        <v>0.99991086591203793</v>
       </c>
       <c r="M3" s="13">
-        <v>0.72251141855881962</v>
+        <v>0.49558944149021678</v>
       </c>
       <c r="P3" s="20">
         <v>80.841999999999999</v>
       </c>
-      <c r="Q3" s="39">
+      <c r="Q3" s="34">
         <v>0.2</v>
       </c>
       <c r="R3" s="30">
@@ -24645,20 +24772,20 @@
       </c>
       <c r="S3" s="28">
         <f>Q3*B14/B13</f>
-        <v>8.2206073727730311E-2</v>
-      </c>
-      <c r="T3" s="45">
+        <v>9.6819535050187894E-2</v>
+      </c>
+      <c r="T3" s="40">
         <f>POWER((R3-P3*W1-X1)/S3,2)</f>
-        <v>14.427612941388384</v>
+        <v>10.712209577508508</v>
       </c>
       <c r="U3" s="5">
         <v>2</v>
       </c>
       <c r="W3" s="13">
-        <v>0.99997470573576774</v>
+        <v>0.99997380964967308</v>
       </c>
       <c r="X3" s="13">
-        <v>0.2639995822163822</v>
+        <v>0.26864006661410622</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
@@ -24672,28 +24799,28 @@
         <v>2</v>
       </c>
       <c r="E4" s="32">
-        <v>123.81</v>
-      </c>
-      <c r="F4" s="60">
-        <v>0.53</v>
-      </c>
-      <c r="G4" s="61">
+        <v>123.48</v>
+      </c>
+      <c r="F4" s="54">
+        <v>0.72</v>
+      </c>
+      <c r="G4" s="55">
         <f>SUM(A3:A5)</f>
         <v>59.370000000000005</v>
       </c>
-      <c r="H4" s="62">
+      <c r="H4" s="56">
         <f>F4*B14/B13</f>
-        <v>0.21784609537848534</v>
-      </c>
-      <c r="I4" s="63">
+        <v>0.34855032618067638</v>
+      </c>
+      <c r="I4" s="57">
         <f>POWER((G4-E4*L1-M1)/H4,2)</f>
-        <v>18.051325346068662</v>
+        <v>4.7845887853442521</v>
       </c>
       <c r="J4" s="5">
         <v>3</v>
       </c>
       <c r="L4" s="13">
-        <v>31665.022554382478</v>
+        <v>67308.314166189928</v>
       </c>
       <c r="M4" s="13">
         <v>6</v>
@@ -24701,7 +24828,7 @@
       <c r="P4" s="20">
         <v>124.02</v>
       </c>
-      <c r="Q4" s="39">
+      <c r="Q4" s="34">
         <v>0.2</v>
       </c>
       <c r="R4" s="30">
@@ -24710,17 +24837,17 @@
       </c>
       <c r="S4" s="25">
         <f>Q4*B14/B13</f>
-        <v>8.2206073727730311E-2</v>
-      </c>
-      <c r="T4" s="45">
+        <v>9.6819535050187894E-2</v>
+      </c>
+      <c r="T4" s="40">
         <f>POWER((R4-P4*W1-X1)/S4,2)</f>
-        <v>9.2612306360068865E-3</v>
+        <v>1.407006268690836E-3</v>
       </c>
       <c r="U4" s="5">
         <v>3</v>
       </c>
       <c r="W4" s="13">
-        <v>237201.92765145932</v>
+        <v>229086.01003825042</v>
       </c>
       <c r="X4" s="13">
         <v>6</v>
@@ -24737,10 +24864,10 @@
         <v>3</v>
       </c>
       <c r="E5" s="6">
-        <v>160.23500000000001</v>
-      </c>
-      <c r="F5" s="69">
-        <v>0.42</v>
+        <v>162.23500000000001</v>
+      </c>
+      <c r="F5" s="6">
+        <v>0.68</v>
       </c>
       <c r="G5" s="4">
         <f>SUM(A3:A6)</f>
@@ -24748,47 +24875,47 @@
       </c>
       <c r="H5" s="6">
         <f>F5*B14/B13</f>
-        <v>0.17263275482823368</v>
-      </c>
-      <c r="I5" s="63">
+        <v>0.32918641917063879</v>
+      </c>
+      <c r="I5" s="40">
         <f>POWER((G5-E5*L1-M1)/H5,2)</f>
-        <v>50.169196318489277</v>
+        <v>0.56529589383419421</v>
       </c>
       <c r="J5" s="5">
         <v>4</v>
       </c>
       <c r="L5" s="13">
-        <v>16529.862151000318</v>
+        <v>16531.520634132907</v>
       </c>
       <c r="M5" s="13">
-        <v>3.1321364996872672</v>
+        <v>1.47365336709951</v>
       </c>
       <c r="P5" s="20">
         <v>166.953</v>
       </c>
-      <c r="Q5" s="39">
+      <c r="Q5" s="34">
         <v>0.2</v>
       </c>
       <c r="R5" s="30">
-        <f>SUM(A2:A5)</f>
-        <v>79.11</v>
+        <f>SUM(A3:A6)</f>
+        <v>79.080000000000013</v>
       </c>
       <c r="S5" s="25">
         <f>Q5*B14/B13</f>
-        <v>8.2206073727730311E-2</v>
-      </c>
-      <c r="T5" s="45">
+        <v>9.6819535050187894E-2</v>
+      </c>
+      <c r="T5" s="40">
         <f>POWER((R5-P5*W1-X1)/S5,2)</f>
-        <v>8.1117869074478541</v>
+        <v>7.222986122067339</v>
       </c>
       <c r="U5" s="5">
         <v>4</v>
       </c>
       <c r="W5" s="13">
-        <v>16531.973225323542</v>
+        <v>16532.561282587663</v>
       </c>
       <c r="X5" s="13">
-        <v>0.41817467646254597</v>
+        <v>0.43300491234258853</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
@@ -24801,23 +24928,23 @@
       <c r="C6" s="5">
         <v>4</v>
       </c>
-      <c r="E6" s="64">
-        <v>202.91</v>
-      </c>
-      <c r="F6" s="65">
-        <v>0.34</v>
-      </c>
-      <c r="G6" s="66">
+      <c r="E6" s="58">
+        <v>202.58</v>
+      </c>
+      <c r="F6" s="66">
+        <v>0.7</v>
+      </c>
+      <c r="G6" s="59">
         <f>SUM(A3:A7)</f>
         <v>98.860000000000014</v>
       </c>
-      <c r="H6" s="67">
+      <c r="H6" s="60">
         <f>F6*B14/B13</f>
-        <v>0.13975032533714155</v>
-      </c>
-      <c r="I6" s="68">
+        <v>0.33886837267565756</v>
+      </c>
+      <c r="I6" s="40">
         <f>POWER((G6-E6*L1-M1)/H6,2)</f>
-        <v>9.368767434816105</v>
+        <v>2.7329612532221161</v>
       </c>
       <c r="J6" s="5">
         <v>5</v>
@@ -24825,7 +24952,7 @@
       <c r="P6" s="20">
         <v>209.47800000000001</v>
       </c>
-      <c r="Q6" s="39">
+      <c r="Q6" s="34">
         <v>0.2</v>
       </c>
       <c r="R6" s="30">
@@ -24834,11 +24961,11 @@
       </c>
       <c r="S6" s="25">
         <f>Q6*B14/B13</f>
-        <v>8.2206073727730311E-2</v>
-      </c>
-      <c r="T6" s="45">
+        <v>9.6819535050187894E-2</v>
+      </c>
+      <c r="T6" s="40">
         <f>POWER((R6-P6*W1-X1)/S6,2)</f>
-        <v>10.050330139642826</v>
+        <v>7.0481118858791989</v>
       </c>
       <c r="U6" s="5">
         <v>5</v>
@@ -24855,37 +24982,37 @@
         <v>5</v>
       </c>
       <c r="E7" s="20">
-        <v>244.69</v>
-      </c>
-      <c r="F7" s="39">
-        <v>0.35</v>
+        <v>244.36</v>
+      </c>
+      <c r="F7" s="67">
+        <v>0.77</v>
       </c>
       <c r="G7" s="30">
         <f>SUM(A3:A8)</f>
         <v>118.82000000000002</v>
       </c>
-      <c r="H7" s="49">
+      <c r="H7" s="44">
         <f>F7*B14/B13</f>
-        <v>0.14386062902352806</v>
-      </c>
-      <c r="I7" s="45">
+        <v>0.37275520994322336</v>
+      </c>
+      <c r="I7" s="40">
         <f>POWER((G7-E7*L1-M1)/H7,2)</f>
-        <v>2.8827251219975025</v>
+        <v>0.93528594894467521</v>
       </c>
       <c r="J7" s="5">
         <v>6</v>
       </c>
       <c r="L7" s="24" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="M7" s="20">
         <f>L1*B13</f>
-        <v>4.7280957582752281</v>
+        <v>4.7319017215916395</v>
       </c>
       <c r="P7" s="20">
         <v>252.197</v>
       </c>
-      <c r="Q7" s="39">
+      <c r="Q7" s="34">
         <v>0.2</v>
       </c>
       <c r="R7" s="30">
@@ -24894,21 +25021,21 @@
       </c>
       <c r="S7" s="25">
         <f>Q7*B14/B13</f>
-        <v>8.2206073727730311E-2</v>
-      </c>
-      <c r="T7" s="45">
+        <v>9.6819535050187894E-2</v>
+      </c>
+      <c r="T7" s="40">
         <f>POWER((R7-P7*W1-X1)/S7,2)</f>
-        <v>4.1423251165223745</v>
+        <v>2.8724375428904176</v>
       </c>
       <c r="U7" s="5">
         <v>6</v>
       </c>
       <c r="W7" s="24" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="X7" s="20">
         <f>W1*B13</f>
-        <v>4.5606258125115007</v>
+        <v>4.5607069245860341</v>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
@@ -24922,37 +25049,37 @@
         <v>6</v>
       </c>
       <c r="E8" s="20">
-        <v>286.55</v>
-      </c>
-      <c r="F8" s="39">
-        <v>0.35</v>
+        <v>286.22000000000003</v>
+      </c>
+      <c r="F8" s="67">
+        <v>0.49</v>
       </c>
       <c r="G8" s="30">
         <f>SUM(A3:A9)</f>
         <v>138.80000000000001</v>
       </c>
-      <c r="H8" s="49">
+      <c r="H8" s="44">
         <f>F8*B14/B13</f>
-        <v>0.14386062902352806</v>
-      </c>
-      <c r="I8" s="45">
+        <v>0.23720786087296031</v>
+      </c>
+      <c r="I8" s="40">
         <f>POWER((G8-E8*L1-M1)/H8,2)</f>
-        <v>8.598907696097316E-2</v>
+        <v>0.35925216873162708</v>
       </c>
       <c r="J8" s="5">
         <v>7</v>
       </c>
-      <c r="L8" s="40" t="s">
-        <v>53</v>
+      <c r="L8" s="35" t="s">
+        <v>51</v>
       </c>
       <c r="M8" s="20">
         <f>L2*B13</f>
-        <v>2.6570294182960381E-2</v>
+        <v>1.8239014116413148E-2</v>
       </c>
       <c r="P8" s="32">
         <v>294.983</v>
       </c>
-      <c r="Q8" s="47">
+      <c r="Q8" s="42">
         <v>0.2</v>
       </c>
       <c r="R8" s="30">
@@ -24961,21 +25088,21 @@
       </c>
       <c r="S8" s="25">
         <f>Q8*B14/B13</f>
-        <v>8.2206073727730311E-2</v>
-      </c>
-      <c r="T8" s="45">
+        <v>9.6819535050187894E-2</v>
+      </c>
+      <c r="T8" s="40">
         <f>POWER((R8-P8*W1-X1)/S8,2)</f>
-        <v>1.0734113773240064</v>
+        <v>0.72264238173568107</v>
       </c>
       <c r="U8" s="5">
         <v>7</v>
       </c>
-      <c r="W8" s="40" t="s">
-        <v>53</v>
+      <c r="W8" s="35" t="s">
+        <v>51</v>
       </c>
       <c r="X8" s="20">
         <f>W2*B13</f>
-        <v>9.3640847133686905E-3</v>
+        <v>9.5286830382847413E-3</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
@@ -24989,33 +25116,33 @@
         <v>7</v>
       </c>
       <c r="E9" s="20">
-        <v>329.36</v>
-      </c>
-      <c r="F9" s="39">
-        <v>0.35</v>
+        <v>329.02</v>
+      </c>
+      <c r="F9" s="67">
+        <v>0.71</v>
       </c>
       <c r="G9" s="30">
         <f>SUM(A3:A10)</f>
         <v>158.76000000000002</v>
       </c>
-      <c r="H9" s="49">
+      <c r="H9" s="44">
         <f>F9*B14/B13</f>
-        <v>0.14386062902352806</v>
-      </c>
-      <c r="I9" s="45">
+        <v>0.34370934942816694</v>
+      </c>
+      <c r="I9" s="40">
         <f>POWER((G9-E9*L1-M1)/H9,2)</f>
-        <v>19.662322431159701</v>
+        <v>2.5578878929653208</v>
       </c>
       <c r="J9" s="5">
         <v>8</v>
       </c>
       <c r="M9" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="P9" s="18">
         <v>336.85700000000003</v>
       </c>
-      <c r="Q9" s="39">
+      <c r="Q9" s="34">
         <v>0.2</v>
       </c>
       <c r="R9" s="30">
@@ -25024,17 +25151,17 @@
       </c>
       <c r="S9" s="25">
         <f>Q9*B14/B13</f>
-        <v>8.2206073727730311E-2</v>
-      </c>
-      <c r="T9" s="45">
+        <v>9.6819535050187894E-2</v>
+      </c>
+      <c r="T9" s="40">
         <f>POWER((R9-P9*W1-X1)/S9,2)</f>
-        <v>23.806835927896977</v>
+        <v>17.378863912824386</v>
       </c>
       <c r="U9" s="5">
         <v>8</v>
       </c>
       <c r="X9" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
@@ -25059,34 +25186,34 @@
         <v>13</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="M11" s="45">
+        <v>63</v>
+      </c>
+      <c r="M11" s="40">
         <f>SUM(I2:I9)</f>
-        <v>103.82683287832106</v>
+        <v>12.725404980104567</v>
       </c>
       <c r="W11" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="X11" s="45">
+        <v>63</v>
+      </c>
+      <c r="X11" s="40">
         <f>SUM(T2:T9)</f>
-        <v>61.879944732368791</v>
+        <v>46.192007590195317</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="L12" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="M12" s="46">
-        <f>7-2</f>
-        <v>5</v>
+        <v>64</v>
+      </c>
+      <c r="M12" s="41">
+        <f>M4</f>
+        <v>6</v>
       </c>
       <c r="W12" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="X12" s="46">
-        <f>7-2</f>
-        <v>5</v>
+        <v>64</v>
+      </c>
+      <c r="X12" s="41">
+        <f>X4</f>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
@@ -25097,68 +25224,68 @@
         <v>9.8066300000000002</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="M13" s="44">
+        <v>65</v>
+      </c>
+      <c r="M13" s="39">
         <f>M11/M12</f>
-        <v>20.76536657566421</v>
+        <v>2.1209008300174279</v>
       </c>
       <c r="W13" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="X13" s="44">
+        <v>65</v>
+      </c>
+      <c r="X13" s="39">
         <f>X11/X12</f>
-        <v>12.375988946473758</v>
+        <v>7.6986679316992195</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="24" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B14" s="25">
-        <v>4.0308227440028599</v>
+        <v>4.7473667850461201</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="L14" s="51" t="s">
-        <v>68</v>
-      </c>
-      <c r="M14" s="52">
+        <v>55</v>
+      </c>
+      <c r="L14" s="46" t="s">
+        <v>66</v>
+      </c>
+      <c r="M14" s="47">
         <f>_xlfn.CHISQ.DIST.RT(M11,M12)</f>
-        <v>8.2425201572806786E-21</v>
-      </c>
-      <c r="W14" s="51" t="s">
-        <v>68</v>
-      </c>
-      <c r="X14" s="52">
+        <v>4.7609799832324891E-2</v>
+      </c>
+      <c r="W14" s="46" t="s">
+        <v>66</v>
+      </c>
+      <c r="X14" s="47">
         <f>_xlfn.CHISQ.DIST.RT(X11,X12)</f>
-        <v>4.9655157569106913E-12</v>
+        <v>2.7110678818943608E-8</v>
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="L15" s="53"/>
+      <c r="L15" s="48"/>
       <c r="M15" s="33"/>
-      <c r="W15" s="53"/>
+      <c r="W15" s="48"/>
       <c r="X15" s="33"/>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="L16" s="53"/>
-      <c r="M16" s="54"/>
-      <c r="W16" s="53"/>
-      <c r="X16" s="54"/>
+      <c r="L16" s="48"/>
+      <c r="M16" s="49"/>
+      <c r="W16" s="48"/>
+      <c r="X16" s="49"/>
     </row>
     <row r="17" spans="12:24" x14ac:dyDescent="0.25">
-      <c r="L17" s="53"/>
-      <c r="M17" s="53"/>
-      <c r="W17" s="53"/>
-      <c r="X17" s="53"/>
+      <c r="L17" s="48"/>
+      <c r="M17" s="48"/>
+      <c r="W17" s="48"/>
+      <c r="X17" s="48"/>
     </row>
     <row r="18" spans="12:24" x14ac:dyDescent="0.25">
-      <c r="L18" s="53"/>
-      <c r="M18" s="55"/>
-      <c r="W18" s="53"/>
-      <c r="X18" s="55"/>
+      <c r="L18" s="48"/>
+      <c r="M18" s="50"/>
+      <c r="W18" s="48"/>
+      <c r="X18" s="50"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -25173,8 +25300,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE2AF99-01D9-4E5D-9BE9-B7536C70F7A1}">
   <dimension ref="A1:Y18"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25196,7 +25323,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E1" s="16" t="s">
         <v>8</v>
@@ -25205,26 +25332,26 @@
         <v>9</v>
       </c>
       <c r="G1" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" s="52" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="K1" s="21" t="s">
         <v>46</v>
-      </c>
-      <c r="H1" s="57" t="s">
-        <v>47</v>
-      </c>
-      <c r="I1" s="48" t="s">
-        <v>71</v>
-      </c>
-      <c r="K1" s="21" t="s">
-        <v>48</v>
       </c>
       <c r="L1" s="13" cm="1">
         <f t="array" ref="L1:M5">LINEST(G2:G8,E2:E8,TRUE,TRUE)</f>
-        <v>0.7792821988029649</v>
+        <v>0.78099273740847042</v>
       </c>
       <c r="M1" s="13">
-        <v>0.67746645489556556</v>
+        <v>0.26230131823486147</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="P1" s="16" t="s">
         <v>8</v>
@@ -25233,26 +25360,26 @@
         <v>9</v>
       </c>
       <c r="R1" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="S1" s="52" t="s">
+        <v>45</v>
+      </c>
+      <c r="T1" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="V1" s="21" t="s">
         <v>46</v>
-      </c>
-      <c r="S1" s="57" t="s">
-        <v>47</v>
-      </c>
-      <c r="T1" s="48" t="s">
-        <v>71</v>
-      </c>
-      <c r="V1" s="21" t="s">
-        <v>48</v>
       </c>
       <c r="W1" s="13" cm="1">
         <f t="array" ref="W1:X5">LINEST(R2:R8,P2:P8,TRUE,TRUE)</f>
-        <v>0.78853232801486228</v>
+        <v>0.79027544870343447</v>
       </c>
       <c r="X1" s="13">
-        <v>-0.23596330210854433</v>
+        <v>-0.39441121735660545</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
@@ -25266,70 +25393,70 @@
         <v>11</v>
       </c>
       <c r="E2" s="19">
-        <v>24.54</v>
-      </c>
-      <c r="F2" s="39">
-        <v>0.2</v>
+        <v>24.87</v>
+      </c>
+      <c r="F2" s="67">
+        <v>0.28999999999999998</v>
       </c>
       <c r="G2" s="30">
-        <f>SUM(A3:A3)</f>
-        <v>19.829999999999998</v>
+        <f>SUM(A4:A4)</f>
+        <v>19.78</v>
       </c>
       <c r="H2" s="18">
         <f>F2*B14/B13</f>
-        <v>0.15752734504474647</v>
-      </c>
-      <c r="I2" s="45">
+        <v>0.22841465031488234</v>
+      </c>
+      <c r="I2" s="40">
         <f>POWER((G2-E2*L1-M1)/H2,2)</f>
-        <v>3.3770447624625673E-2</v>
+        <v>0.17083689360644147</v>
       </c>
       <c r="J2" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K2" s="21" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L2" s="13">
-        <v>4.5015506745775214E-3</v>
+        <v>4.7611787454765481E-3</v>
       </c>
       <c r="M2" s="13">
-        <v>0.50805271849695166</v>
+        <v>0.53877155022166701</v>
       </c>
       <c r="N2" s="23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="P2" s="20">
         <v>25.337</v>
       </c>
-      <c r="Q2" s="39">
+      <c r="Q2" s="34">
         <v>0.2</v>
       </c>
       <c r="R2" s="30">
-        <f>SUM(A3:A3)</f>
-        <v>19.829999999999998</v>
+        <f>SUM(A4:A4)</f>
+        <v>19.78</v>
       </c>
       <c r="S2" s="25">
         <f>Q2*B14/B13</f>
         <v>0.15752734504474647</v>
       </c>
-      <c r="T2" s="45">
+      <c r="T2" s="40">
         <f>POWER((R2-P2*W1-X1)/S2,2)</f>
-        <v>0.30445604561983464</v>
+        <v>0.92130655586505639</v>
       </c>
       <c r="U2" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V2" s="21" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="W2" s="13">
-        <v>2.3991653999091891E-3</v>
+        <v>2.7646389646880012E-3</v>
       </c>
       <c r="X2" s="13">
-        <v>0.27008476764767486</v>
+        <v>0.31122775963496724</v>
       </c>
       <c r="Y2" s="23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -25343,58 +25470,58 @@
         <v>1</v>
       </c>
       <c r="E3" s="20">
-        <v>50.16</v>
-      </c>
-      <c r="F3" s="18">
-        <v>0.39</v>
+        <v>50.49</v>
+      </c>
+      <c r="F3" s="67">
+        <v>0.47</v>
       </c>
       <c r="G3" s="30">
-        <f>SUM(A3:A4)</f>
-        <v>39.61</v>
+        <f>SUM(A4:A5)</f>
+        <v>39.540000000000006</v>
       </c>
       <c r="H3" s="29">
         <f>F3*B14/B13</f>
-        <v>0.3071783228372556</v>
-      </c>
-      <c r="I3" s="45">
+        <v>0.37018926085515419</v>
+      </c>
+      <c r="I3" s="40">
         <f>POWER((G3-E3*L1-M1)/H3,2)</f>
-        <v>0.25877547148530267</v>
+        <v>0.1744655625904083</v>
       </c>
       <c r="J3" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L3" s="13">
-        <v>0.99983318606493321</v>
+        <v>0.99981420916326358</v>
       </c>
       <c r="M3" s="13">
-        <v>0.60562756521223216</v>
+        <v>0.64056593437519871</v>
       </c>
       <c r="P3" s="20">
         <v>50.503</v>
       </c>
-      <c r="Q3" s="39">
+      <c r="Q3" s="34">
         <v>0.2</v>
       </c>
       <c r="R3" s="30">
-        <f>SUM(A3:A4)</f>
-        <v>39.61</v>
+        <f>SUM(A4:A5)</f>
+        <v>39.540000000000006</v>
       </c>
       <c r="S3" s="28">
         <f>Q3*B14/B13</f>
         <v>0.15752734504474647</v>
       </c>
-      <c r="T3" s="45">
+      <c r="T3" s="40">
         <f>POWER((R3-P3*W1-X1)/S3,2)</f>
-        <v>2.0793085673370959E-2</v>
+        <v>2.1559964996243203E-2</v>
       </c>
       <c r="U3" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="W3" s="13">
-        <v>0.99995371595834204</v>
+        <v>0.99993881241684723</v>
       </c>
       <c r="X3" s="13">
-        <v>0.31901059576977303</v>
+        <v>0.36760663656070991</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
@@ -25408,28 +25535,28 @@
         <v>2</v>
       </c>
       <c r="E4" s="20">
-        <v>74.790000000000006</v>
-      </c>
-      <c r="F4" s="18">
-        <v>0.27</v>
+        <v>75.13</v>
+      </c>
+      <c r="F4" s="67">
+        <v>0.38</v>
       </c>
       <c r="G4" s="30">
-        <f>SUM(A3:A5)</f>
-        <v>59.370000000000005</v>
+        <f>SUM(A4:A6)</f>
+        <v>59.250000000000007</v>
       </c>
       <c r="H4" s="18">
         <f>F4*B14/B13</f>
-        <v>0.21266191581040775</v>
-      </c>
-      <c r="I4" s="45">
+        <v>0.29930195558501826</v>
+      </c>
+      <c r="I4" s="40">
         <f>POWER((G4-E4*L1-M1)/H4,2)</f>
-        <v>3.7172877696020117</v>
+        <v>1.0846619362726488</v>
       </c>
       <c r="J4" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L4" s="13">
-        <v>29968.51509031374</v>
+        <v>26906.983862236404</v>
       </c>
       <c r="M4" s="13">
         <v>5</v>
@@ -25437,26 +25564,26 @@
       <c r="P4" s="20">
         <v>75.704999999999998</v>
       </c>
-      <c r="Q4" s="39">
+      <c r="Q4" s="34">
         <v>0.2</v>
       </c>
       <c r="R4" s="30">
-        <f>SUM(A3:A5)</f>
-        <v>59.370000000000005</v>
+        <f>SUM(A4:A6)</f>
+        <v>59.250000000000007</v>
       </c>
       <c r="S4" s="25">
         <f>Q4*B14/B13</f>
         <v>0.15752734504474647</v>
       </c>
-      <c r="T4" s="45">
+      <c r="T4" s="40">
         <f>POWER((R4-P4*W1-X1)/S4,2)</f>
-        <v>0.32552269212313634</v>
+        <v>1.3553363889130894</v>
       </c>
       <c r="U4" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="W4" s="13">
-        <v>108023.5951894474</v>
+        <v>81710.925721762003</v>
       </c>
       <c r="X4" s="13">
         <v>5</v>
@@ -25473,58 +25600,58 @@
         <v>3</v>
       </c>
       <c r="E5" s="20">
-        <v>101.83</v>
-      </c>
-      <c r="F5" s="18">
-        <v>0.41</v>
+        <v>102.16</v>
+      </c>
+      <c r="F5" s="67">
+        <v>0.49</v>
       </c>
       <c r="G5" s="30">
-        <f>SUM(A3:A6)</f>
-        <v>79.080000000000013</v>
+        <f>SUM(A4:A7)</f>
+        <v>79.03</v>
       </c>
       <c r="H5" s="18">
         <f>F5*B14/B13</f>
-        <v>0.32293105734173022</v>
-      </c>
-      <c r="I5" s="45">
+        <v>0.38594199535962881</v>
+      </c>
+      <c r="I5" s="40">
         <f>POWER((G5-E5*L1-M1)/H5,2)</f>
-        <v>8.6865417633491635</v>
+        <v>6.9645732647383793</v>
       </c>
       <c r="J5" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L5" s="13">
-        <v>10991.99424768985</v>
+        <v>11040.600519275733</v>
       </c>
       <c r="M5" s="13">
-        <v>1.8339237387244829</v>
+        <v>2.0516235814098565</v>
       </c>
       <c r="P5" s="20">
         <v>101.09699999999999</v>
       </c>
-      <c r="Q5" s="39">
+      <c r="Q5" s="34">
         <v>0.2</v>
       </c>
       <c r="R5" s="30">
-        <f>SUM(A3:A6)</f>
-        <v>79.080000000000013</v>
+        <f>SUM(A4:A7)</f>
+        <v>79.03</v>
       </c>
       <c r="S5" s="25">
         <f>Q5*B14/B13</f>
         <v>0.15752734504474647</v>
       </c>
-      <c r="T5" s="45">
+      <c r="T5" s="40">
         <f>POWER((R5-P5*W1-X1)/S5,2)</f>
-        <v>6.5217689430315398</v>
+        <v>8.9044159760080657</v>
       </c>
       <c r="U5" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="W5" s="13">
-        <v>10993.319332627509</v>
+        <v>11041.976469660925</v>
       </c>
       <c r="X5" s="13">
-        <v>0.50883880106692758</v>
+        <v>0.67567319621738942</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
@@ -25538,46 +25665,46 @@
         <v>4</v>
       </c>
       <c r="E6" s="20">
-        <v>125.11</v>
-      </c>
-      <c r="F6" s="39">
-        <v>0.2</v>
+        <v>125.44</v>
+      </c>
+      <c r="F6" s="67">
+        <v>0.28000000000000003</v>
       </c>
       <c r="G6" s="30">
-        <f>SUM(A3:A7)</f>
-        <v>98.860000000000014</v>
+        <f>SUM(A4:A8)</f>
+        <v>98.990000000000009</v>
       </c>
       <c r="H6" s="18">
         <f>F6*B14/B13</f>
-        <v>0.15752734504474647</v>
-      </c>
-      <c r="I6" s="45">
+        <v>0.22053828306264506</v>
+      </c>
+      <c r="I6" s="40">
         <f>POWER((G6-E6*L1-M1)/H6,2)</f>
-        <v>18.994016671000594</v>
+        <v>11.874752802978525</v>
       </c>
       <c r="J6" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P6" s="20">
         <v>124.98099999999999</v>
       </c>
-      <c r="Q6" s="39">
+      <c r="Q6" s="34">
         <v>0.2</v>
       </c>
       <c r="R6" s="30">
-        <f>SUM(A3:A7)</f>
-        <v>98.860000000000014</v>
+        <f>SUM(A4:A8)</f>
+        <v>98.990000000000009</v>
       </c>
       <c r="S6" s="25">
         <f>Q6*B14/B13</f>
         <v>0.15752734504474647</v>
       </c>
-      <c r="T6" s="45">
+      <c r="T6" s="40">
         <f>POWER((R6-P6*W1-X1)/S6,2)</f>
-        <v>11.943493274481074</v>
+        <v>15.241642662036167</v>
       </c>
       <c r="U6" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
@@ -25591,60 +25718,60 @@
         <v>5</v>
       </c>
       <c r="E7" s="20">
-        <v>151.15</v>
-      </c>
-      <c r="F7" s="39">
-        <v>0.2</v>
+        <v>151.49</v>
+      </c>
+      <c r="F7" s="67">
+        <v>0.28999999999999998</v>
       </c>
       <c r="G7" s="30">
-        <f>SUM(A3:A8)</f>
-        <v>118.82000000000002</v>
+        <f>SUM(A4:A9)</f>
+        <v>118.97000000000001</v>
       </c>
       <c r="H7" s="18">
         <f>F7*B14/B13</f>
-        <v>0.15752734504474647</v>
-      </c>
-      <c r="I7" s="45">
+        <v>0.22841465031488234</v>
+      </c>
+      <c r="I7" s="40">
         <f>POWER((G7-E7*L1-M1)/H7,2)</f>
-        <v>5.050870697484326</v>
+        <v>2.9921660799094338</v>
       </c>
       <c r="J7" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L7" s="24" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="M7" s="20">
         <f>L1*B13</f>
-        <v>7.6421321892471195</v>
+        <v>7.658906808452028</v>
       </c>
       <c r="P7" s="32">
         <v>151.21799999999999</v>
       </c>
-      <c r="Q7" s="47">
+      <c r="Q7" s="42">
         <v>0.2</v>
       </c>
       <c r="R7" s="30">
-        <f>SUM(A3:A8)</f>
-        <v>118.82000000000002</v>
+        <f>SUM(A4:A9)</f>
+        <v>118.97000000000001</v>
       </c>
       <c r="S7" s="25">
         <f>Q7*B14/B13</f>
         <v>0.15752734504474647</v>
       </c>
-      <c r="T7" s="45">
+      <c r="T7" s="40">
         <f>POWER((R7-P7*W1-X1)/S7,2)</f>
-        <v>1.369067593434605</v>
+        <v>0.78378560764525129</v>
       </c>
       <c r="U7" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="W7" s="24" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="X7" s="20">
         <f>W1*B13</f>
-        <v>7.7328447838803891</v>
+        <v>7.7499389235185614</v>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
@@ -25658,60 +25785,60 @@
         <v>6</v>
       </c>
       <c r="E8" s="20">
-        <v>177.72</v>
-      </c>
-      <c r="F8" s="39">
-        <v>0.2</v>
+        <v>178.05</v>
+      </c>
+      <c r="F8" s="67">
+        <v>0.28999999999999998</v>
       </c>
       <c r="G8" s="30">
-        <f>SUM(A3:A9)</f>
-        <v>138.80000000000001</v>
+        <f>SUM(A4:A10)</f>
+        <v>138.93</v>
       </c>
       <c r="H8" s="18">
         <f>F8*B14/B13</f>
-        <v>0.15752734504474647</v>
-      </c>
-      <c r="I8" s="45">
+        <v>0.22841465031488234</v>
+      </c>
+      <c r="I8" s="40">
         <f>POWER((G8-E8*L1-M1)/H8,2)</f>
-        <v>5.5616414181254061</v>
+        <v>2.8863291083853202</v>
       </c>
       <c r="J8" s="5">
-        <v>7</v>
-      </c>
-      <c r="L8" s="40" t="s">
-        <v>53</v>
+        <v>8</v>
+      </c>
+      <c r="L8" s="35" t="s">
+        <v>51</v>
       </c>
       <c r="M8" s="20">
         <f>L2*B13</f>
-        <v>4.414504189183216E-2</v>
+        <v>4.6691118320752685E-2</v>
       </c>
       <c r="P8" s="18">
         <v>176.29400000000001</v>
       </c>
-      <c r="Q8" s="39">
+      <c r="Q8" s="34">
         <v>0.2</v>
       </c>
       <c r="R8" s="30">
-        <f>SUM(A3:A9)</f>
-        <v>138.80000000000001</v>
+        <f>SUM(A4:A10)</f>
+        <v>138.93</v>
       </c>
       <c r="S8" s="25">
         <f>Q8*B14/B13</f>
         <v>0.15752734504474647</v>
       </c>
-      <c r="T8" s="45">
+      <c r="T8" s="40">
         <f>POWER((R8-P8*W1-X1)/S8,2)</f>
-        <v>2.0301583208275693E-2</v>
+        <v>5.1973584288023263E-4</v>
       </c>
       <c r="U8" s="5">
-        <v>7</v>
-      </c>
-      <c r="W8" s="40" t="s">
-        <v>53</v>
+        <v>8</v>
+      </c>
+      <c r="W8" s="35" t="s">
+        <v>51</v>
       </c>
       <c r="X8" s="20">
         <f>W2*B13</f>
-        <v>2.3527727385711451E-2</v>
+        <v>2.7111791410278294E-2</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
@@ -25725,10 +25852,10 @@
         <v>7</v>
       </c>
       <c r="M9" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="X9" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
@@ -25753,33 +25880,33 @@
         <v>17</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="M11" s="45">
+        <v>63</v>
+      </c>
+      <c r="M11" s="40">
         <f>SUM(I2:I8)</f>
-        <v>42.302904238671431</v>
+        <v>26.147785648481161</v>
       </c>
       <c r="W11" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="X11" s="45">
+        <v>63</v>
+      </c>
+      <c r="X11" s="40">
         <f>SUM(T2:T8)</f>
-        <v>20.505403217571835</v>
+        <v>27.228566891306748</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="L12" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="M12" s="46">
-        <f>7-2</f>
+        <v>64</v>
+      </c>
+      <c r="M12" s="41">
+        <f>M4</f>
         <v>5</v>
       </c>
       <c r="W12" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="X12" s="46">
-        <f>7-2</f>
+        <v>64</v>
+      </c>
+      <c r="X12" s="41">
+        <f>X4</f>
         <v>5</v>
       </c>
     </row>
@@ -25791,75 +25918,72 @@
         <v>9.8066300000000002</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="M13" s="44">
+        <v>65</v>
+      </c>
+      <c r="M13" s="39">
         <f>M11/M12</f>
-        <v>8.4605808477342865</v>
+        <v>5.2295571296962322</v>
       </c>
       <c r="W13" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="X13" s="44">
+        <v>65</v>
+      </c>
+      <c r="X13" s="39">
         <f>X11/X12</f>
-        <v>4.1010806435143667</v>
+        <v>5.4457133782613498</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="24" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B14" s="25">
         <v>7.7240619386808103</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="L14" s="51" t="s">
-        <v>68</v>
-      </c>
-      <c r="M14" s="52">
+        <v>55</v>
+      </c>
+      <c r="L14" s="46" t="s">
+        <v>66</v>
+      </c>
+      <c r="M14" s="47">
         <f>_xlfn.CHISQ.DIST.RT(M11,M12)</f>
-        <v>5.1148781474451658E-8</v>
-      </c>
-      <c r="W14" s="51" t="s">
-        <v>68</v>
-      </c>
-      <c r="X14" s="52">
+        <v>8.3535226722442909E-5</v>
+      </c>
+      <c r="W14" s="46" t="s">
+        <v>66</v>
+      </c>
+      <c r="X14" s="47">
         <f>_xlfn.CHISQ.DIST.RT(X11,X12)</f>
-        <v>1.0041724501660585E-3</v>
+        <v>5.1483510371567872E-5</v>
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="L15" s="53"/>
+      <c r="L15" s="48"/>
       <c r="M15" s="33"/>
-      <c r="W15" s="53"/>
+      <c r="W15" s="48"/>
       <c r="X15" s="33"/>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="L16" s="53"/>
-      <c r="M16" s="54"/>
-      <c r="W16" s="53"/>
-      <c r="X16" s="54"/>
+      <c r="L16" s="48"/>
+      <c r="M16" s="49"/>
+      <c r="W16" s="48"/>
+      <c r="X16" s="49"/>
     </row>
     <row r="17" spans="12:24" x14ac:dyDescent="0.25">
-      <c r="L17" s="53"/>
-      <c r="M17" s="53"/>
-      <c r="W17" s="53"/>
-      <c r="X17" s="53"/>
+      <c r="L17" s="48"/>
+      <c r="M17" s="48"/>
+      <c r="W17" s="48"/>
+      <c r="X17" s="48"/>
     </row>
     <row r="18" spans="12:24" x14ac:dyDescent="0.25">
-      <c r="L18" s="53"/>
-      <c r="M18" s="56"/>
-      <c r="W18" s="53"/>
-      <c r="X18" s="56"/>
+      <c r="L18" s="48"/>
+      <c r="M18" s="51"/>
+      <c r="W18" s="48"/>
+      <c r="X18" s="51"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="G3:G7" formulaRange="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -25867,15 +25991,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF0B04D7-4CCB-4FB2-B94F-F6D78953706E}">
   <dimension ref="A1:Y21"/>
   <sheetViews>
-    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+    <sheetView topLeftCell="A3" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="4.5703125" customWidth="1"/>
     <col min="7" max="7" width="2.28515625" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" customWidth="1"/>
+    <col min="8" max="9" width="9.140625" customWidth="1"/>
     <col min="11" max="11" width="9" customWidth="1"/>
     <col min="13" max="13" width="4.5703125" customWidth="1"/>
     <col min="14" max="14" width="2.28515625" customWidth="1"/>
@@ -25895,17 +26019,17 @@
       <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="51" t="s">
+      <c r="E1" s="46" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="I1" s="38" t="s">
         <v>60</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="I1" s="43" t="s">
-        <v>62</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>0</v>
@@ -25913,11 +26037,11 @@
       <c r="K1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="48" t="s">
-        <v>71</v>
+      <c r="L1" s="43" t="s">
+        <v>69</v>
       </c>
       <c r="N1" s="21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="O1" s="13" cm="1">
         <f t="array" ref="O1:P5">LINEST(J2:J10,H2:H10,TRUE,TRUE)</f>
@@ -25927,7 +26051,7 @@
         <v>6.2051326557669597</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="V1" s="8"/>
       <c r="W1" s="8"/>
@@ -25956,7 +26080,7 @@
         <v>6.6098221957829328E-3</v>
       </c>
       <c r="I2" s="9">
-        <f t="shared" ref="I2:I10" si="1">2*F2/POWER(E2,3)</f>
+        <f>2*F2/POWER(E2,3)</f>
         <v>1.0351541014107014E-4</v>
       </c>
       <c r="J2" s="4">
@@ -25965,17 +26089,17 @@
       </c>
       <c r="K2" s="4">
         <f>I2*B15*1000</f>
-        <v>0.41725226955140982</v>
-      </c>
-      <c r="L2" s="45">
+        <v>0.49142561984414268</v>
+      </c>
+      <c r="L2" s="40">
         <f>POWER((J2-H2*O1-P1)/K2,2)</f>
-        <v>12.04407690294326</v>
+        <v>8.6827110174804165</v>
       </c>
       <c r="M2" s="5">
         <v>0</v>
       </c>
       <c r="N2" s="21" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="O2" s="13">
         <v>44.103646025853088</v>
@@ -25984,10 +26108,10 @@
         <v>1.1063071197276355</v>
       </c>
       <c r="Q2" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="V2" s="58"/>
-      <c r="W2" s="58"/>
+        <v>49</v>
+      </c>
+      <c r="V2" s="53"/>
+      <c r="W2" s="53"/>
       <c r="X2" s="7"/>
       <c r="Y2" s="7"/>
     </row>
@@ -26005,7 +26129,7 @@
         <v>9.64</v>
       </c>
       <c r="F3" s="6">
-        <f t="shared" ref="F3:F10" si="2">POWER(E3,2)*(1/250)/(2*PI())</f>
+        <f t="shared" ref="F3:F10" si="1">POWER(E3,2)*(1/250)/(2*PI())</f>
         <v>5.9160820798210396E-2</v>
       </c>
       <c r="H3" s="9">
@@ -26013,20 +26137,20 @@
         <v>1.0760834007678931E-2</v>
       </c>
       <c r="I3" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="I3:I10" si="2">2*F3/POWER(E3,3)</f>
         <v>1.3207879094763098E-4</v>
       </c>
-      <c r="J3" s="41">
+      <c r="J3" s="36">
         <f>SUM(A11,A2:A3)</f>
         <v>60.29</v>
       </c>
       <c r="K3" s="4">
         <f>I3*B15*1000</f>
-        <v>0.53238619455211</v>
-      </c>
-      <c r="L3" s="45">
+        <v>0.62702646515383342</v>
+      </c>
+      <c r="L3" s="40">
         <f>POWER((J3-H3*O1-P1)/K3,2)</f>
-        <v>1.608288983449788</v>
+        <v>1.1594336858210648</v>
       </c>
       <c r="M3" s="5">
         <v>1</v>
@@ -26037,8 +26161,8 @@
       <c r="P3" s="13">
         <v>1.3645886683994108</v>
       </c>
-      <c r="V3" s="58"/>
-      <c r="W3" s="58"/>
+      <c r="V3" s="53"/>
+      <c r="W3" s="53"/>
       <c r="X3" s="7"/>
       <c r="Y3" s="7"/>
     </row>
@@ -26064,7 +26188,7 @@
         <v>1.4944913050495874E-2</v>
       </c>
       <c r="I4" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.5565275608009328E-4</v>
       </c>
       <c r="J4" s="29">
@@ -26073,11 +26197,11 @@
       </c>
       <c r="K4" s="4">
         <f>I4*B15*1000</f>
-        <v>0.62740866937436934</v>
-      </c>
-      <c r="L4" s="45">
+        <v>0.73894072421552037</v>
+      </c>
+      <c r="L4" s="40">
         <f>POWER((J4-H4*O1-P1)/K4,2)</f>
-        <v>0.24705913621233619</v>
+        <v>0.17810772060379557</v>
       </c>
       <c r="M4" s="5">
         <v>2</v>
@@ -26088,8 +26212,8 @@
       <c r="P4" s="13">
         <v>7</v>
       </c>
-      <c r="V4" s="58"/>
-      <c r="W4" s="58"/>
+      <c r="V4" s="53"/>
+      <c r="W4" s="53"/>
       <c r="X4" s="7"/>
       <c r="Y4" s="7"/>
     </row>
@@ -26107,7 +26231,7 @@
         <v>7.24</v>
       </c>
       <c r="F5" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3.3370080580054931E-2</v>
       </c>
       <c r="H5" s="9">
@@ -26115,20 +26239,20 @@
         <v>1.9077561734989774E-2</v>
       </c>
       <c r="I5" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.7586181557115507E-4</v>
       </c>
-      <c r="J5" s="42">
+      <c r="J5" s="37">
         <f>SUM(A11,A2:A5)</f>
         <v>99.83</v>
       </c>
       <c r="K5" s="4">
         <f>I5*B15*1000</f>
-        <v>0.7088678060058482</v>
-      </c>
-      <c r="L5" s="45">
+        <v>0.83488054200040818</v>
+      </c>
+      <c r="L5" s="40">
         <f>POWER((J5-H5*O1-P1)/K5,2)</f>
-        <v>2.2512808970858815</v>
+        <v>1.6229738157678106</v>
       </c>
       <c r="M5" s="5">
         <v>3</v>
@@ -26139,8 +26263,8 @@
       <c r="P5" s="13">
         <v>13.034715637468542</v>
       </c>
-      <c r="V5" s="58"/>
-      <c r="W5" s="58"/>
+      <c r="V5" s="53"/>
+      <c r="W5" s="53"/>
       <c r="X5" s="7"/>
       <c r="Y5" s="7"/>
     </row>
@@ -26158,7 +26282,7 @@
         <v>6.58</v>
       </c>
       <c r="F6" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2.7563344312335748E-2</v>
       </c>
       <c r="H6" s="9">
@@ -26166,7 +26290,7 @@
         <v>2.3096608494008741E-2</v>
       </c>
       <c r="I6" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.9350145056765391E-4</v>
       </c>
       <c r="J6" s="4">
@@ -26175,17 +26299,17 @@
       </c>
       <c r="K6" s="4">
         <f>I6*B15*1000</f>
-        <v>0.77997004794564451</v>
-      </c>
-      <c r="L6" s="45">
+        <v>0.91862235928312386</v>
+      </c>
+      <c r="L6" s="40">
         <f>POWER((J6-H6*O1-P1)/K6,2)</f>
-        <v>2.7844468457349474</v>
+        <v>2.0073391676155192</v>
       </c>
       <c r="M6" s="5">
         <v>4</v>
       </c>
-      <c r="V6" s="58"/>
-      <c r="W6" s="58"/>
+      <c r="V6" s="53"/>
+      <c r="W6" s="53"/>
       <c r="X6" s="7"/>
       <c r="Y6" s="7"/>
     </row>
@@ -26203,7 +26327,7 @@
         <v>6.07</v>
       </c>
       <c r="F7" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2.3456191850906302E-2</v>
       </c>
       <c r="H7" s="9">
@@ -26211,7 +26335,7 @@
         <v>2.7140798319441765E-2</v>
       </c>
       <c r="I7" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.097593978146891E-4</v>
       </c>
       <c r="J7" s="4">
@@ -26220,33 +26344,33 @@
       </c>
       <c r="K7" s="4">
         <f>I7*B15*1000</f>
-        <v>0.84550295147979271</v>
-      </c>
-      <c r="L7" s="45">
+        <v>0.99580479803673072</v>
+      </c>
+      <c r="L7" s="40">
         <f>POWER((J7-H7*O1-P1)/K7,2)</f>
-        <v>3.555167330015558</v>
+        <v>2.5629602662009798</v>
       </c>
       <c r="M7" s="5">
         <v>5</v>
       </c>
       <c r="O7" s="24" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="P7" s="20">
         <f>O1*0.001</f>
         <v>4.963342432735943</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="S7" s="45">
+        <v>63</v>
+      </c>
+      <c r="S7" s="40">
         <f>POWER((J2-H2*O1-P1)/K2,2)+POWER((J3-H3*O1-P1)/K3,2)+POWER((J4-H4*O1-P1)/K4,2)+POWER((J5-H5*O1-P1)/K5,2)+POWER((J6-H6*O1-P1)/K6,2)+POWER((J7-H7*O1-P1)/K7,2)+POWER((J8-H8*O1-P1)/K8,2)+POWER((J9-H9*O1-P1)/K9,2)+POWER((J10-H10*O1-P1)/K10,2)</f>
-        <v>27.481498396625668</v>
-      </c>
-      <c r="T7" s="53"/>
+        <v>19.811722461431732</v>
+      </c>
+      <c r="T7" s="48"/>
       <c r="U7" s="33"/>
-      <c r="V7" s="58"/>
-      <c r="W7" s="58"/>
+      <c r="V7" s="53"/>
+      <c r="W7" s="53"/>
       <c r="X7" s="7"/>
       <c r="Y7" s="7"/>
     </row>
@@ -26264,7 +26388,7 @@
         <v>5.7</v>
       </c>
       <c r="F8" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2.0683776404222722E-2</v>
       </c>
       <c r="H8" s="9">
@@ -26272,7 +26396,7 @@
         <v>3.077870113881194E-2</v>
       </c>
       <c r="I8" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.2337535872546716E-4</v>
       </c>
       <c r="J8" s="4">
@@ -26281,33 +26405,33 @@
       </c>
       <c r="K8" s="4">
         <f>I8*B15*1000</f>
-        <v>0.9003864764004107</v>
-      </c>
-      <c r="L8" s="45">
+        <v>1.0604447586110448</v>
+      </c>
+      <c r="L8" s="40">
         <f>POWER((J8-H8*O1-P1)/K8,2)</f>
-        <v>0.11826037189797788</v>
+        <v>8.5255237265960598E-2</v>
       </c>
       <c r="M8" s="5">
         <v>6</v>
       </c>
-      <c r="O8" s="40" t="s">
-        <v>53</v>
+      <c r="O8" s="35" t="s">
+        <v>51</v>
       </c>
       <c r="P8" s="20">
         <f>O2*0.001</f>
         <v>4.4103646025853087E-2</v>
       </c>
       <c r="R8" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="S8" s="46">
-        <f>9-2</f>
+        <v>64</v>
+      </c>
+      <c r="S8" s="41">
+        <f>P4</f>
         <v>7</v>
       </c>
-      <c r="T8" s="53"/>
-      <c r="U8" s="54"/>
-      <c r="V8" s="58"/>
-      <c r="W8" s="58"/>
+      <c r="T8" s="48"/>
+      <c r="U8" s="49"/>
+      <c r="V8" s="53"/>
+      <c r="W8" s="53"/>
       <c r="X8" s="7"/>
       <c r="Y8" s="7"/>
     </row>
@@ -26325,7 +26449,7 @@
         <v>5.35</v>
       </c>
       <c r="F9" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.8221649434591095E-2</v>
       </c>
       <c r="H9" s="9">
@@ -26333,7 +26457,7 @@
         <v>3.4937549130928475E-2</v>
       </c>
       <c r="I9" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.3798869995049775E-4</v>
       </c>
       <c r="J9" s="4">
@@ -26342,26 +26466,26 @@
       </c>
       <c r="K9" s="4">
         <f>I9*B15*1000</f>
-        <v>0.95929026457613853</v>
-      </c>
-      <c r="L9" s="45">
+        <v>1.1298196493613002</v>
+      </c>
+      <c r="L9" s="40">
         <f>POWER((J9-H9*O1-P1)/K9,2)</f>
-        <v>0.13476034122757366</v>
+        <v>9.7150251441032856E-2</v>
       </c>
       <c r="M9" s="5">
         <v>7</v>
       </c>
       <c r="R9" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="S9" s="44">
+        <v>65</v>
+      </c>
+      <c r="S9" s="39">
         <f>S7/S8</f>
-        <v>3.9259283423750952</v>
-      </c>
-      <c r="T9" s="53"/>
-      <c r="U9" s="53"/>
-      <c r="V9" s="58"/>
-      <c r="W9" s="58"/>
+        <v>2.8302460659188187</v>
+      </c>
+      <c r="T9" s="48"/>
+      <c r="U9" s="48"/>
+      <c r="V9" s="53"/>
+      <c r="W9" s="53"/>
       <c r="X9" s="7"/>
       <c r="Y9" s="7"/>
     </row>
@@ -26379,7 +26503,7 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="F10" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.655848027928079E-2</v>
       </c>
       <c r="H10" s="9">
@@ -26387,7 +26511,7 @@
         <v>3.844675124951942E-2</v>
       </c>
       <c r="I10" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.496548126931692E-4</v>
       </c>
       <c r="J10" s="4">
@@ -26396,26 +26520,26 @@
       </c>
       <c r="K10" s="4">
         <f>I10*B15*1000</f>
-        <v>1.0063142971534003</v>
-      </c>
-      <c r="L10" s="45">
+        <v>1.185202965506462</v>
+      </c>
+      <c r="L10" s="40">
         <f>POWER((J10-H10*O1-P1)/K10,2)</f>
-        <v>4.7381575880583453</v>
+        <v>3.4157912992351505</v>
       </c>
       <c r="M10" s="5">
         <v>8</v>
       </c>
-      <c r="R10" s="51" t="s">
-        <v>68</v>
-      </c>
-      <c r="S10" s="52">
+      <c r="R10" s="46" t="s">
+        <v>66</v>
+      </c>
+      <c r="S10" s="47">
         <f>_xlfn.CHISQ.DIST.RT(S7,S8)</f>
-        <v>2.7290008748132445E-4</v>
-      </c>
-      <c r="T10" s="53"/>
-      <c r="U10" s="56"/>
-      <c r="V10" s="58"/>
-      <c r="W10" s="58"/>
+        <v>5.9910425569618432E-3</v>
+      </c>
+      <c r="T10" s="48"/>
+      <c r="U10" s="51"/>
+      <c r="V10" s="53"/>
+      <c r="W10" s="53"/>
       <c r="X10" s="7"/>
       <c r="Y10" s="7"/>
     </row>
@@ -26444,16 +26568,16 @@
         <v>14</v>
       </c>
       <c r="E12" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H12" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="I12" s="38" t="s">
         <v>60</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="I12" s="43" t="s">
-        <v>62</v>
       </c>
       <c r="J12" s="3" t="s">
         <v>0</v>
@@ -26461,11 +26585,11 @@
       <c r="K12" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="L12" s="48" t="s">
-        <v>71</v>
+      <c r="L12" s="43" t="s">
+        <v>69</v>
       </c>
       <c r="N12" s="21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="O12" s="13" cm="1">
         <f t="array" ref="O12:P16">LINEST(J13:J20,H13:H20,TRUE,TRUE)</f>
@@ -26475,7 +26599,7 @@
         <v>15.245024783120471</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
@@ -26502,7 +26626,7 @@
         <f>I13*B16*1000</f>
         <v>0.83343907680611462</v>
       </c>
-      <c r="L13" s="45">
+      <c r="L13" s="40">
         <f>POWER((J13-H13*O12-P12)/K13,2)</f>
         <v>9.4792512811135016E-3</v>
       </c>
@@ -26510,7 +26634,7 @@
         <v>1</v>
       </c>
       <c r="N13" s="21" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="O13" s="13">
         <v>23.444715674728755</v>
@@ -26519,7 +26643,7 @@
         <v>0.40454850284847993</v>
       </c>
       <c r="Q13" s="23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
@@ -26552,7 +26676,7 @@
         <f>I14*B16*1000</f>
         <v>0.97372090161506464</v>
       </c>
-      <c r="L14" s="45">
+      <c r="L14" s="40">
         <f>POWER((J14-H14*O12-P12)/K14,2)</f>
         <v>0.17665413967763091</v>
       </c>
@@ -26568,13 +26692,13 @@
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="24" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B15" s="25">
-        <v>4.0308227440028599</v>
+        <v>4.7473667850461201</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E15" s="6">
         <v>9.02</v>
@@ -26599,7 +26723,7 @@
         <f>I15*B16*1000</f>
         <v>1.0903083266421458</v>
       </c>
-      <c r="L15" s="45">
+      <c r="L15" s="40">
         <f>POWER((J15-H15*O12-P12)/K15,2)</f>
         <v>5.8452381472819753E-2</v>
       </c>
@@ -26615,13 +26739,13 @@
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" s="24" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B16" s="25">
         <v>7.7240619386808103</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E16" s="6">
         <v>8.2200000000000006</v>
@@ -26646,7 +26770,7 @@
         <f>I16*B16*1000</f>
         <v>1.1964210591620625</v>
       </c>
-      <c r="L16" s="45">
+      <c r="L16" s="40">
         <f>POWER((J16-H16*O12-P12)/K16,2)</f>
         <v>0.36916656973521561</v>
       </c>
@@ -26684,7 +26808,7 @@
         <f>I17*B16*1000</f>
         <v>1.3008705167079568</v>
       </c>
-      <c r="L17" s="45">
+      <c r="L17" s="40">
         <f>POWER((J17-H17*O12-P12)/K17,2)</f>
         <v>1.9682712028665134E-2</v>
       </c>
@@ -26716,7 +26840,7 @@
         <f>I18*B16*1000</f>
         <v>1.3949760434485328</v>
       </c>
-      <c r="L18" s="45">
+      <c r="L18" s="40">
         <f>POWER((J18-H18*O12-P12)/K18,2)</f>
         <v>6.119458476283722E-2</v>
       </c>
@@ -26724,20 +26848,20 @@
         <v>6</v>
       </c>
       <c r="O18" s="24" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="P18" s="20">
         <f>O12*0.001</f>
         <v>7.6715837559065019</v>
       </c>
       <c r="R18" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="S18" s="45">
+        <v>63</v>
+      </c>
+      <c r="S18" s="40">
         <f>POWER((J13-H13*O12-P12)/K13,2)+POWER((J14-H14*O12-P12)/K14,2)+POWER((J15-H15*O12-P12)/K15,2)+POWER((J16-H16*O12-P12)/K16,2)+POWER((J17-H17*O12-P12)/K17,2)+POWER((J18-H18*O12-P12)/K18,2)+POWER((J19-H19*O12-P12)/K19,2)+POWER((J20-H20*O12-P12)/K20,2)</f>
         <v>0.69546336439227519</v>
       </c>
-      <c r="T18" s="53"/>
+      <c r="T18" s="48"/>
       <c r="U18" s="33"/>
     </row>
     <row r="19" spans="5:21" x14ac:dyDescent="0.25">
@@ -26764,29 +26888,29 @@
         <f>I19*B16*1000</f>
         <v>1.4811116123964088</v>
       </c>
-      <c r="L19" s="45">
+      <c r="L19" s="40">
         <f>POWER((J19-H19*O12-P12)/K19,2)</f>
         <v>1.0085213846702314E-4</v>
       </c>
       <c r="M19" s="5">
         <v>7</v>
       </c>
-      <c r="O19" s="40" t="s">
-        <v>53</v>
+      <c r="O19" s="35" t="s">
+        <v>51</v>
       </c>
       <c r="P19" s="20">
         <f>O13*0.001</f>
         <v>2.3444715674728757E-2</v>
       </c>
       <c r="R19" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="S19" s="46">
-        <f>8-2</f>
+        <v>64</v>
+      </c>
+      <c r="S19" s="41">
+        <f>P15</f>
         <v>6</v>
       </c>
-      <c r="T19" s="53"/>
-      <c r="U19" s="54"/>
+      <c r="T19" s="48"/>
+      <c r="U19" s="49"/>
     </row>
     <row r="20" spans="5:21" x14ac:dyDescent="0.25">
       <c r="E20" s="6">
@@ -26812,7 +26936,7 @@
         <f>I20*B16*1000</f>
         <v>1.5635264079987525</v>
       </c>
-      <c r="L20" s="45">
+      <c r="L20" s="40">
         <f>POWER((J20-H20*O12-P12)/K20,2)</f>
         <v>7.3287329552602822E-4</v>
       </c>
@@ -26820,25 +26944,25 @@
         <v>8</v>
       </c>
       <c r="R20" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="S20" s="44">
+        <v>65</v>
+      </c>
+      <c r="S20" s="39">
         <f>S18/S19</f>
         <v>0.11591056073204586</v>
       </c>
-      <c r="T20" s="53"/>
-      <c r="U20" s="53"/>
+      <c r="T20" s="48"/>
+      <c r="U20" s="48"/>
     </row>
     <row r="21" spans="5:21" x14ac:dyDescent="0.25">
-      <c r="R21" s="51" t="s">
-        <v>68</v>
-      </c>
-      <c r="S21" s="52">
+      <c r="R21" s="46" t="s">
+        <v>66</v>
+      </c>
+      <c r="S21" s="47">
         <f>_xlfn.CHISQ.DIST.RT(S18,S19)</f>
         <v>0.99458844909941413</v>
       </c>
-      <c r="T21" s="53"/>
-      <c r="U21" s="56"/>
+      <c r="T21" s="48"/>
+      <c r="U21" s="51"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>